<commit_message>
Removed FlexWilliams (requires further testing), added TraPPE C15 and C16 annealing
</commit_message>
<xml_diff>
--- a/simulation_plans_results.xlsx
+++ b/simulation_plans_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Dropbox\Github_Dropbox\AlkaneStudy.Gromacs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D45611-8741-4620-BEC7-D44FA2812F20}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F991ABC3-6B2C-4F96-A482-E3B22A80BB80}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EF8A33E0-ACA8-D640-B463-6863C93E9688}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="207">
   <si>
     <t>Study</t>
   </si>
@@ -635,28 +635,55 @@
     </r>
   </si>
   <si>
-    <t>Tests performed (if needed)</t>
-  </si>
-  <si>
     <t>Flex-Williams 4T</t>
   </si>
   <si>
     <t>COMPASS</t>
   </si>
   <si>
-    <t>Sim notes</t>
-  </si>
-  <si>
     <t>Force field notes</t>
   </si>
   <si>
-    <t>Should test parameter versions 4 and 7</t>
-  </si>
-  <si>
-    <t>Also test with and without C-H bond constraints</t>
-  </si>
-  <si>
     <t>GPU</t>
+  </si>
+  <si>
+    <t>COMPASS 9-6</t>
+  </si>
+  <si>
+    <t>Trying to simplify COMPASS for Gromacs is probably a bad idea,</t>
+  </si>
+  <si>
+    <t>better to use the 9-6 non-bonded potential with a standard harmonic+dihedral bonding potential.</t>
+  </si>
+  <si>
+    <t>Tests performed</t>
+  </si>
+  <si>
+    <t>Outstanding problems</t>
+  </si>
+  <si>
+    <t>FlexWilliams</t>
+  </si>
+  <si>
+    <t>Simulation notes</t>
+  </si>
+  <si>
+    <t>Should test parameter versions 4 and 7.</t>
+  </si>
+  <si>
+    <t>Also test with and without C-H bond constraints.</t>
+  </si>
+  <si>
+    <t>After correcting bonding parameters, C16 now freezes at 298K so can't measure properties.</t>
+  </si>
+  <si>
+    <t>Box volume fluctuates wildly - maybe a resonance effect.</t>
+  </si>
+  <si>
+    <t>Try Lincs version, untabulated version, or shorter cutoffs (Williams used &lt;0.7 nm)</t>
+  </si>
+  <si>
+    <t>Try changing time constant of pressure couping. Check FF parameters.</t>
   </si>
 </sst>
 </file>
@@ -669,7 +696,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -755,13 +782,26 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -858,7 +898,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1062,6 +1102,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2527,10 +2572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E6099B-77F6-4CCD-9B30-DB7CF2E469C9}">
-  <dimension ref="B2:O23"/>
+  <dimension ref="B2:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2544,19 +2589,19 @@
     <col min="12" max="12" width="27.5" style="19" customWidth="1"/>
     <col min="13" max="13" width="17.625" style="19" customWidth="1"/>
     <col min="14" max="14" width="32.5" style="19" customWidth="1"/>
-    <col min="15" max="15" width="56.625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="65.625" style="19" customWidth="1"/>
     <col min="16" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15">
+    <row r="2" spans="2:12">
       <c r="H2" s="19" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="2:15" s="20" customFormat="1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" s="20" customFormat="1">
       <c r="D3" s="20" t="s">
         <v>177</v>
       </c>
@@ -2570,7 +2615,7 @@
         <v>180</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>182</v>
@@ -2578,11 +2623,8 @@
       <c r="K3" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="N3" s="20" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" ht="15.75" customHeight="1">
+    </row>
+    <row r="4" spans="2:12" ht="15.75" customHeight="1">
       <c r="B4" s="19" t="s">
         <v>44</v>
       </c>
@@ -2602,7 +2644,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" s="19">
         <v>2</v>
@@ -2613,11 +2655,8 @@
       <c r="L4" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="N4" s="70" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15">
+    </row>
+    <row r="5" spans="2:12">
       <c r="C5" s="19" t="s">
         <v>189</v>
       </c>
@@ -2634,7 +2673,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="19">
         <v>0</v>
@@ -2645,11 +2684,8 @@
       <c r="L5" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="N5" s="19" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15">
+    </row>
+    <row r="6" spans="2:12">
       <c r="C6" s="19" t="s">
         <v>176</v>
       </c>
@@ -2675,13 +2711,10 @@
         <v>2</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7" s="19" t="s">
         <v>43</v>
       </c>
@@ -2695,13 +2728,13 @@
         <v>3</v>
       </c>
       <c r="F7" s="19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" s="19">
         <v>0</v>
       </c>
       <c r="H7" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="19">
         <v>0</v>
@@ -2713,7 +2746,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:12">
       <c r="C8" s="19" t="s">
         <v>189</v>
       </c>
@@ -2721,7 +2754,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8" s="19">
         <v>3</v>
@@ -2742,7 +2775,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:12">
       <c r="C9" s="19" t="s">
         <v>176</v>
       </c>
@@ -2765,7 +2798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:12">
       <c r="B10" s="19" t="s">
         <v>35</v>
       </c>
@@ -2791,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:12">
       <c r="C11" s="19" t="s">
         <v>189</v>
       </c>
@@ -2814,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:12">
       <c r="C12" s="19" t="s">
         <v>176</v>
       </c>
@@ -2837,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:15" s="20" customFormat="1">
+    <row r="14" spans="2:12" s="20" customFormat="1">
       <c r="D14" s="20" t="s">
         <v>177</v>
       </c>
@@ -2851,49 +2884,37 @@
         <v>180</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="N14" s="20" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15">
+    </row>
+    <row r="15" spans="2:12">
       <c r="B15" s="19" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="N15" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="O15" s="19" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15">
+    </row>
+    <row r="16" spans="2:12">
       <c r="C16" s="19" t="s">
         <v>189</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="O16" s="19" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
       <c r="C17" s="19" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:12">
       <c r="B18" s="19" t="s">
         <v>43</v>
       </c>
@@ -2901,23 +2922,23 @@
         <v>183</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:12">
       <c r="C19" s="19" t="s">
         <v>189</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
       <c r="C20" s="19" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:12">
       <c r="B21" s="19" t="s">
         <v>35</v>
       </c>
@@ -2925,21 +2946,175 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:12">
       <c r="C22" s="19" t="s">
         <v>189</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
       <c r="C23" s="19" t="s">
         <v>176</v>
       </c>
+    </row>
+    <row r="27" spans="2:12" s="20" customFormat="1">
+      <c r="C27" s="73" t="s">
+        <v>192</v>
+      </c>
+      <c r="L27" s="73" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="C28" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" s="71" t="s">
+        <v>201</v>
+      </c>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="L28" s="70" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="D29" t="s">
+        <v>202</v>
+      </c>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="L29" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="C30" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="D30" t="s">
+        <v>195</v>
+      </c>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="L30" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12">
+      <c r="D31" t="s">
+        <v>196</v>
+      </c>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+    </row>
+    <row r="32" spans="2:12">
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+    </row>
+    <row r="33" spans="3:12">
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="3:12">
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+    </row>
+    <row r="35" spans="3:12">
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+    </row>
+    <row r="36" spans="3:12" s="20" customFormat="1">
+      <c r="C36" s="73" t="s">
+        <v>198</v>
+      </c>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="72"/>
+    </row>
+    <row r="37" spans="3:12">
+      <c r="C37" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="D37" s="50" t="s">
+        <v>203</v>
+      </c>
+      <c r="L37" s="50" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12">
+      <c r="C38" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D38" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="L38" s="50" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12">
+      <c r="D39" s="50"/>
+      <c r="L39" s="50"/>
+    </row>
+    <row r="40" spans="3:12">
+      <c r="D40" s="50"/>
+      <c r="L40" s="50"/>
+    </row>
+    <row r="41" spans="3:12">
+      <c r="D41" s="50"/>
+      <c r="L41" s="50"/>
+    </row>
+    <row r="42" spans="3:12">
+      <c r="D42" s="50"/>
+      <c r="L42" s="50"/>
+    </row>
+    <row r="43" spans="3:12">
+      <c r="D43" s="50"/>
+      <c r="L43" s="50"/>
+    </row>
+    <row r="44" spans="3:12">
+      <c r="L44" s="50"/>
+    </row>
+    <row r="45" spans="3:12">
+      <c r="L45" s="50"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K4:K9">
@@ -5855,8 +6030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDAA431D-5536-2842-8755-AEE6B34A948B}">
   <dimension ref="B2:AA17"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Z18" sqref="Z18"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Z26" sqref="Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Added Williams potential scan for C8, fixed some .itp filenames
</commit_message>
<xml_diff>
--- a/simulation_plans_results.xlsx
+++ b/simulation_plans_results.xlsx
@@ -1,6 +1,49 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Dropbox\github_dropbox\alkanestudy.gromacs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EB5834-9D33-427E-A8BD-4DD7A0B3033C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{EF8A33E0-ACA8-D640-B463-6863C93E9688}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sim matrix" sheetId="13" r:id="rId1"/>
+    <sheet name="Outline" sheetId="1" r:id="rId2"/>
+    <sheet name="PYS-W" sheetId="6" r:id="rId3"/>
+    <sheet name="Sun9-6" sheetId="9" r:id="rId4"/>
+    <sheet name="FlexWilliams" sheetId="10" r:id="rId5"/>
+    <sheet name="WilliamsOpt" sheetId="14" r:id="rId6"/>
+    <sheet name="CHARMM36" sheetId="11" r:id="rId7"/>
+    <sheet name="box_sizes" sheetId="5" r:id="rId8"/>
+    <sheet name="cos-acc tests" sheetId="7" r:id="rId9"/>
+    <sheet name="Expr data" sheetId="2" r:id="rId10"/>
+    <sheet name="Ref" sheetId="3" r:id="rId11"/>
+    <sheet name="Expr old" sheetId="4" state="hidden" r:id="rId12"/>
+  </sheets>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
+</workbook>
+</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="253">
   <si>
     <t>Study</t>
   </si>
@@ -780,6 +823,30 @@
   </si>
   <si>
     <t>FlexWilliams4L-OPLS_rc0.6_1024xC16_properties_298K_1bar</t>
+  </si>
+  <si>
+    <t>Δε</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>L (sim)</t>
+  </si>
+  <si>
+    <t>D - FSC</t>
+  </si>
+  <si>
+    <t>FSC = finite size correction</t>
+  </si>
+  <si>
+    <t>Phase 1</t>
+  </si>
+  <si>
+    <t>Phase 2</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1096,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1279,6 +1346,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3393,6 +3470,1454 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB14C90-9A0C-E346-B9BD-40AE56D235C4}">
+  <dimension ref="B1:BH46"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AP15" sqref="AP15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="5" style="4" customWidth="1"/>
+    <col min="2" max="4" width="7.875" style="4"/>
+    <col min="5" max="5" width="7.875" style="7"/>
+    <col min="6" max="7" width="7.875" style="4"/>
+    <col min="8" max="12" width="3.625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="5" style="4" customWidth="1"/>
+    <col min="14" max="19" width="7.875" style="4"/>
+    <col min="20" max="24" width="3.625" style="10" customWidth="1"/>
+    <col min="25" max="25" width="5" style="4" customWidth="1"/>
+    <col min="26" max="28" width="7.875" style="4"/>
+    <col min="29" max="29" width="7.875" style="7"/>
+    <col min="30" max="30" width="7.875" style="8"/>
+    <col min="31" max="31" width="7.875" style="4"/>
+    <col min="32" max="36" width="3.625" style="10" customWidth="1"/>
+    <col min="37" max="37" width="5" style="4" customWidth="1"/>
+    <col min="38" max="39" width="7.875" style="4"/>
+    <col min="40" max="40" width="7.875" style="12"/>
+    <col min="41" max="41" width="7.875" style="4"/>
+    <col min="42" max="42" width="7.875" style="8"/>
+    <col min="43" max="43" width="7.875" style="4"/>
+    <col min="44" max="48" width="3.625" style="10" customWidth="1"/>
+    <col min="49" max="49" width="5" style="4" customWidth="1"/>
+    <col min="50" max="53" width="7.875" style="4"/>
+    <col min="54" max="54" width="7.875" style="8"/>
+    <col min="55" max="55" width="7.875" style="4"/>
+    <col min="56" max="60" width="3.625" style="10" customWidth="1"/>
+    <col min="61" max="16384" width="7.875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:55" ht="15" customHeight="1">
+      <c r="Z1" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="2:55" ht="15" customHeight="1">
+      <c r="B2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="N2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="Z2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA2" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB2" s="84"/>
+      <c r="AC2" s="84"/>
+      <c r="AD2" s="84"/>
+      <c r="AE2" s="84"/>
+      <c r="AL2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM2" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN2" s="84"/>
+      <c r="AO2" s="84"/>
+      <c r="AP2" s="84"/>
+      <c r="AQ2" s="84"/>
+      <c r="AY2" s="86" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ2" s="86"/>
+      <c r="BA2" s="15"/>
+      <c r="BB2" s="15"/>
+      <c r="BC2" s="15"/>
+    </row>
+    <row r="3" spans="2:55" ht="15" customHeight="1">
+      <c r="B3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4">
+        <v>25</v>
+      </c>
+      <c r="G3" s="4">
+        <v>30</v>
+      </c>
+      <c r="H3" s="10">
+        <v>10</v>
+      </c>
+      <c r="I3" s="10">
+        <v>15</v>
+      </c>
+      <c r="J3" s="10">
+        <v>20</v>
+      </c>
+      <c r="K3" s="10">
+        <v>25</v>
+      </c>
+      <c r="L3" s="10">
+        <v>30</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="4">
+        <v>10</v>
+      </c>
+      <c r="P3" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>20</v>
+      </c>
+      <c r="R3" s="4">
+        <v>25</v>
+      </c>
+      <c r="S3" s="4">
+        <v>30</v>
+      </c>
+      <c r="T3" s="10">
+        <v>10</v>
+      </c>
+      <c r="U3" s="10">
+        <v>15</v>
+      </c>
+      <c r="V3" s="10">
+        <v>20</v>
+      </c>
+      <c r="W3" s="10">
+        <v>25</v>
+      </c>
+      <c r="X3" s="10">
+        <v>30</v>
+      </c>
+      <c r="Z3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>10</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>15</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>20</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE3" s="4">
+        <v>30</v>
+      </c>
+      <c r="AF3" s="10">
+        <v>10</v>
+      </c>
+      <c r="AG3" s="10">
+        <v>15</v>
+      </c>
+      <c r="AH3" s="10">
+        <v>20</v>
+      </c>
+      <c r="AI3" s="10">
+        <v>25</v>
+      </c>
+      <c r="AJ3" s="10">
+        <v>30</v>
+      </c>
+      <c r="AL3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM3" s="4">
+        <v>10</v>
+      </c>
+      <c r="AN3" s="4">
+        <v>15</v>
+      </c>
+      <c r="AO3" s="4">
+        <v>20</v>
+      </c>
+      <c r="AP3" s="4">
+        <v>25</v>
+      </c>
+      <c r="AQ3" s="4">
+        <v>30</v>
+      </c>
+      <c r="AR3" s="10">
+        <v>10</v>
+      </c>
+      <c r="AS3" s="10">
+        <v>15</v>
+      </c>
+      <c r="AT3" s="10">
+        <v>20</v>
+      </c>
+      <c r="AU3" s="10">
+        <v>25</v>
+      </c>
+      <c r="AV3" s="10">
+        <v>30</v>
+      </c>
+      <c r="AY3" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AZ3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="BB3" s="4"/>
+    </row>
+    <row r="4" spans="2:55" ht="15" customHeight="1">
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="7">
+        <v>635.9</v>
+      </c>
+      <c r="D4" s="7">
+        <v>631.04</v>
+      </c>
+      <c r="E4" s="7">
+        <v>626.12</v>
+      </c>
+      <c r="F4" s="7">
+        <v>621.14</v>
+      </c>
+      <c r="G4" s="7">
+        <v>616.11</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="12"/>
+      <c r="Z4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>17.149999999999999</v>
+      </c>
+      <c r="AC4" s="7">
+        <v>16.05</v>
+      </c>
+      <c r="AD4" s="63">
+        <f>0.5*(AC4+AE4)</f>
+        <v>15.495000000000001</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>14.94</v>
+      </c>
+      <c r="AF4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
+      <c r="AQ4" s="8"/>
+      <c r="AX4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AY4" s="4">
+        <v>143.5</v>
+      </c>
+      <c r="AZ4" s="18">
+        <f t="shared" ref="AZ4:AZ15" si="0">AY4-273.15</f>
+        <v>-129.64999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="2:55" ht="15" customHeight="1">
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="7">
+        <v>668.37</v>
+      </c>
+      <c r="D5" s="7">
+        <v>663.91</v>
+      </c>
+      <c r="E5" s="7">
+        <v>659.42</v>
+      </c>
+      <c r="F5" s="7">
+        <v>654.89</v>
+      </c>
+      <c r="G5" s="7">
+        <v>650.33000000000004</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="12">
+        <v>0.2949</v>
+      </c>
+      <c r="W5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>19.420000000000002</v>
+      </c>
+      <c r="AC5" s="7">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="AD5" s="63">
+        <f t="shared" ref="AD5:AD15" si="1">0.5*(AC5+AE5)</f>
+        <v>17.89</v>
+      </c>
+      <c r="AE5" s="4">
+        <v>17.38</v>
+      </c>
+      <c r="AF5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM5" s="8"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8"/>
+      <c r="AQ5" s="8"/>
+      <c r="AX5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AY5" s="4">
+        <v>177.8</v>
+      </c>
+      <c r="AZ5" s="18">
+        <f t="shared" si="0"/>
+        <v>-95.349999999999966</v>
+      </c>
+    </row>
+    <row r="6" spans="2:55" ht="15" customHeight="1">
+      <c r="B6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="7">
+        <v>692.4</v>
+      </c>
+      <c r="D6" s="7">
+        <v>688.2</v>
+      </c>
+      <c r="E6" s="7">
+        <v>683.99</v>
+      </c>
+      <c r="F6" s="7">
+        <v>679.75</v>
+      </c>
+      <c r="G6" s="7">
+        <v>675.49</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="12">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="W6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA6" s="7">
+        <v>21.12</v>
+      </c>
+      <c r="AC6" s="7">
+        <v>20.14</v>
+      </c>
+      <c r="AD6" s="63">
+        <f t="shared" si="1"/>
+        <v>19.655000000000001</v>
+      </c>
+      <c r="AE6" s="4">
+        <v>19.170000000000002</v>
+      </c>
+      <c r="AF6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM6" s="8"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="8"/>
+      <c r="AQ6" s="8"/>
+      <c r="AX6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AY6" s="4">
+        <v>182.6</v>
+      </c>
+      <c r="AZ6" s="18">
+        <f t="shared" si="0"/>
+        <v>-90.549999999999983</v>
+      </c>
+    </row>
+    <row r="7" spans="2:55" ht="15" customHeight="1">
+      <c r="B7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="N7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="12">
+        <v>0.50919999999999999</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA7" s="7">
+        <v>22.57</v>
+      </c>
+      <c r="AC7" s="7">
+        <v>21.62</v>
+      </c>
+      <c r="AD7" s="63">
+        <f t="shared" si="1"/>
+        <v>21.145000000000003</v>
+      </c>
+      <c r="AE7" s="4">
+        <v>20.67</v>
+      </c>
+      <c r="AF7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM7" s="8"/>
+      <c r="AN7" s="8">
+        <v>1.988</v>
+      </c>
+      <c r="AO7" s="8">
+        <v>2.14</v>
+      </c>
+      <c r="AP7" s="8">
+        <v>2.3559999999999999</v>
+      </c>
+      <c r="AQ7" s="8">
+        <v>2.633</v>
+      </c>
+      <c r="AS7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AY7" s="4">
+        <v>216.4</v>
+      </c>
+      <c r="AZ7" s="18">
+        <f t="shared" si="0"/>
+        <v>-56.749999999999972</v>
+      </c>
+    </row>
+    <row r="8" spans="2:55" ht="15" customHeight="1">
+      <c r="B8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="N8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="12"/>
+      <c r="Z8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA8" s="7">
+        <v>23.79</v>
+      </c>
+      <c r="AC8" s="7">
+        <v>22.85</v>
+      </c>
+      <c r="AD8" s="63">
+        <f t="shared" si="1"/>
+        <v>22.385000000000002</v>
+      </c>
+      <c r="AE8" s="4">
+        <v>21.92</v>
+      </c>
+      <c r="AF8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM8" s="8"/>
+      <c r="AN8" s="8">
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="AO8" s="8">
+        <v>1.6259999999999999</v>
+      </c>
+      <c r="AP8" s="8">
+        <v>1.772</v>
+      </c>
+      <c r="AQ8" s="8">
+        <v>1.9610000000000001</v>
+      </c>
+      <c r="AS8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AY8" s="4">
+        <v>219.7</v>
+      </c>
+      <c r="AZ8" s="18">
+        <f t="shared" si="0"/>
+        <v>-53.449999999999989</v>
+      </c>
+    </row>
+    <row r="9" spans="2:55" ht="15" customHeight="1">
+      <c r="B9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="N9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="12">
+        <v>0.8498</v>
+      </c>
+      <c r="W9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA9" s="7">
+        <v>24.75</v>
+      </c>
+      <c r="AC9" s="7">
+        <v>23.83</v>
+      </c>
+      <c r="AD9" s="63">
+        <f t="shared" si="1"/>
+        <v>23.369999999999997</v>
+      </c>
+      <c r="AE9" s="4">
+        <v>22.91</v>
+      </c>
+      <c r="AF9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM9" s="8"/>
+      <c r="AN9" s="8">
+        <v>1.165</v>
+      </c>
+      <c r="AO9" s="8">
+        <v>1.268</v>
+      </c>
+      <c r="AP9" s="8">
+        <v>1.3859999999999999</v>
+      </c>
+      <c r="AQ9" s="8">
+        <v>1.5589999999999999</v>
+      </c>
+      <c r="AS9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY9" s="4">
+        <v>243.5</v>
+      </c>
+      <c r="AZ9" s="18">
+        <f t="shared" si="0"/>
+        <v>-29.649999999999977</v>
+      </c>
+    </row>
+    <row r="10" spans="2:55" ht="15" customHeight="1">
+      <c r="B10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="N10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="12"/>
+      <c r="Z10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA10" s="7">
+        <v>25.56</v>
+      </c>
+      <c r="AC10" s="7">
+        <v>24.66</v>
+      </c>
+      <c r="AD10" s="63">
+        <f t="shared" si="1"/>
+        <v>24.21</v>
+      </c>
+      <c r="AE10" s="4">
+        <v>23.76</v>
+      </c>
+      <c r="AF10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM10" s="8"/>
+      <c r="AN10" s="8">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="AO10" s="8">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="AP10" s="8">
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="AQ10" s="8">
+        <v>1.248</v>
+      </c>
+      <c r="AS10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AY10" s="4">
+        <v>247.6</v>
+      </c>
+      <c r="AZ10" s="18">
+        <f t="shared" si="0"/>
+        <v>-25.549999999999983</v>
+      </c>
+    </row>
+    <row r="11" spans="2:55" ht="15" customHeight="1">
+      <c r="B11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="N11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="12">
+        <v>1.3585</v>
+      </c>
+      <c r="W11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA11" s="7">
+        <v>26.24</v>
+      </c>
+      <c r="AC11" s="7">
+        <v>25.35</v>
+      </c>
+      <c r="AD11" s="63">
+        <f t="shared" si="1"/>
+        <v>24.91</v>
+      </c>
+      <c r="AE11" s="4">
+        <v>24.47</v>
+      </c>
+      <c r="AF11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM11" s="8"/>
+      <c r="AN11" s="8">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="AO11" s="8">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="AP11" s="8">
+        <v>0.871</v>
+      </c>
+      <c r="AQ11" s="8">
+        <v>0.996</v>
+      </c>
+      <c r="AS11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AY11" s="4">
+        <v>263.60000000000002</v>
+      </c>
+      <c r="AZ11" s="18">
+        <f t="shared" si="0"/>
+        <v>-9.5499999999999545</v>
+      </c>
+    </row>
+    <row r="12" spans="2:55" ht="15" customHeight="1">
+      <c r="B12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="N12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="12"/>
+      <c r="Z12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA12" s="7">
+        <v>26.86</v>
+      </c>
+      <c r="AC12" s="7">
+        <v>25.99</v>
+      </c>
+      <c r="AD12" s="63">
+        <f t="shared" si="1"/>
+        <v>25.549999999999997</v>
+      </c>
+      <c r="AE12" s="4">
+        <v>25.11</v>
+      </c>
+      <c r="AF12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM12" s="8"/>
+      <c r="AN12" s="8">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="AO12" s="8">
+        <v>0.64</v>
+      </c>
+      <c r="AP12" s="8">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AQ12" s="8">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="AS12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY12" s="4">
+        <v>267.8</v>
+      </c>
+      <c r="AZ12" s="18">
+        <f t="shared" si="0"/>
+        <v>-5.3499999999999659</v>
+      </c>
+    </row>
+    <row r="13" spans="2:55" ht="15" customHeight="1">
+      <c r="B13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="N13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="12">
+        <v>2.0779999999999998</v>
+      </c>
+      <c r="W13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA13" s="7">
+        <v>27.43</v>
+      </c>
+      <c r="AC13" s="7">
+        <v>26.56</v>
+      </c>
+      <c r="AD13" s="63">
+        <f t="shared" si="1"/>
+        <v>26.125</v>
+      </c>
+      <c r="AE13" s="4">
+        <v>25.69</v>
+      </c>
+      <c r="AF13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM13" s="8"/>
+      <c r="AN13" s="8">
+        <v>0.443</v>
+      </c>
+      <c r="AO13" s="8">
+        <v>0.495</v>
+      </c>
+      <c r="AP13" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AQ13" s="8">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="AS13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AY13" s="4">
+        <v>279</v>
+      </c>
+      <c r="AZ13" s="18">
+        <f t="shared" si="0"/>
+        <v>5.8500000000000227</v>
+      </c>
+    </row>
+    <row r="14" spans="2:55" ht="15" customHeight="1">
+      <c r="B14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="N14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q14" s="7"/>
+      <c r="Z14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC14" s="7">
+        <v>27.07</v>
+      </c>
+      <c r="AD14" s="63">
+        <f t="shared" si="1"/>
+        <v>26.64</v>
+      </c>
+      <c r="AE14" s="4">
+        <v>26.21</v>
+      </c>
+      <c r="AH14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM14" s="8"/>
+      <c r="AN14" s="8">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="AO14" s="8">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="AP14" s="8">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="AQ14" s="8">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="AS14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AY14" s="4">
+        <v>283.10000000000002</v>
+      </c>
+      <c r="AZ14" s="18">
+        <f t="shared" si="0"/>
+        <v>9.9500000000000455</v>
+      </c>
+    </row>
+    <row r="15" spans="2:55" ht="15" customHeight="1">
+      <c r="B15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="N15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q15" s="7"/>
+      <c r="Z15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC15" s="7">
+        <v>27.47</v>
+      </c>
+      <c r="AD15" s="63">
+        <f t="shared" si="1"/>
+        <v>27.045000000000002</v>
+      </c>
+      <c r="AE15" s="4">
+        <v>26.62</v>
+      </c>
+      <c r="AH15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM15" s="8"/>
+      <c r="AN15" s="16"/>
+      <c r="AO15" s="8">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="AP15" s="8">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="AQ15" s="8">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="AT15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AY15" s="4">
+        <v>291.10000000000002</v>
+      </c>
+      <c r="AZ15" s="18">
+        <f t="shared" si="0"/>
+        <v>17.950000000000045</v>
+      </c>
+    </row>
+    <row r="16" spans="2:55" ht="15" customHeight="1">
+      <c r="Q16" s="7"/>
+      <c r="AM16" s="8"/>
+      <c r="AN16" s="16"/>
+      <c r="AO16" s="8"/>
+      <c r="AQ16" s="8"/>
+    </row>
+    <row r="17" spans="2:43" ht="15" customHeight="1">
+      <c r="Q17" s="7"/>
+      <c r="AM17" s="8"/>
+      <c r="AN17" s="16"/>
+      <c r="AO17" s="8"/>
+      <c r="AQ17" s="8"/>
+    </row>
+    <row r="18" spans="2:43" ht="15" customHeight="1">
+      <c r="B18" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="84"/>
+    </row>
+    <row r="19" spans="2:43" ht="15" customHeight="1">
+      <c r="B19" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="4">
+        <v>10</v>
+      </c>
+      <c r="D19" s="4">
+        <v>15</v>
+      </c>
+      <c r="E19" s="4">
+        <v>20</v>
+      </c>
+      <c r="F19" s="4">
+        <v>25</v>
+      </c>
+      <c r="G19" s="4">
+        <v>30</v>
+      </c>
+      <c r="H19" s="10">
+        <v>10</v>
+      </c>
+      <c r="I19" s="10">
+        <v>15</v>
+      </c>
+      <c r="J19" s="10">
+        <v>20</v>
+      </c>
+      <c r="K19" s="10">
+        <v>25</v>
+      </c>
+      <c r="L19" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:43" ht="15" customHeight="1">
+      <c r="B20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7">
+        <v>626.20000000000005</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="J20" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:43" ht="15" customHeight="1">
+      <c r="B21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="F21" s="7">
+        <v>660.6</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="K21" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:43" ht="15" customHeight="1">
+      <c r="B22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="F22" s="7">
+        <v>679.5</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="K22" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="2:43" ht="15" customHeight="1">
+      <c r="B23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="F23" s="7">
+        <v>698.6</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="K23" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="2:43" ht="15" customHeight="1">
+      <c r="B24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7">
+        <v>719.2</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="J24" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:43" ht="15" customHeight="1">
+      <c r="B25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="F25" s="7">
+        <v>726.6</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="K25" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:43" ht="15" customHeight="1">
+      <c r="B26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7">
+        <v>740.2</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="J26" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="2:43" ht="15" customHeight="1">
+      <c r="B27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7">
+        <v>749.5</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="J27" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="2:43" ht="15" customHeight="1">
+      <c r="B28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7">
+        <v>756.4</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="J28" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="2:43" ht="15" customHeight="1">
+      <c r="B29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7">
+        <v>759.6</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="J29" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:43" ht="15" customHeight="1">
+      <c r="B30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7">
+        <v>768.5</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="J30" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="2:43" ht="15" customHeight="1">
+      <c r="B31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="F31" s="7">
+        <v>770.1</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="K31" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="6:14" ht="15" customHeight="1">
+      <c r="F33" s="5"/>
+    </row>
+    <row r="46" spans="6:14" ht="15" customHeight="1">
+      <c r="N46" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="AY2:AZ2"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="AM2:AQ2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BDCE98-34D0-4ABF-8516-E6ECC928D09D}">
   <dimension ref="B2:C32"/>
   <sheetViews>
@@ -3606,7 +5131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C044A9FB-F8D3-4917-BFAB-FBE43DD433AF}">
   <dimension ref="B3:BH17"/>
   <sheetViews>
@@ -6301,11 +7826,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDAA431D-5536-2842-8755-AEE6B34A948B}">
   <dimension ref="B2:AC50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D41" sqref="D41"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -7577,6 +9102,317 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2C844C-ED1A-4540-A821-8B893B2A81D6}">
+  <dimension ref="B1:K43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="9" style="19"/>
+    <col min="2" max="2" width="17.5" style="19" customWidth="1"/>
+    <col min="3" max="3" width="9" style="19"/>
+    <col min="4" max="4" width="9" style="34"/>
+    <col min="5" max="16384" width="9" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11">
+      <c r="G1" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11">
+      <c r="E2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="J2" s="50" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="C4" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="C5" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="C7" s="81" t="s">
+        <v>251</v>
+      </c>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="H7" s="81" t="s">
+        <v>252</v>
+      </c>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="90"/>
+    </row>
+    <row r="8" spans="2:11" s="20" customFormat="1">
+      <c r="D8" s="89" t="s">
+        <v>245</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="88" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="89" t="s">
+        <v>245</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="88" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="34">
+        <v>0.01</v>
+      </c>
+      <c r="H9" s="19">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="D10" s="34">
+        <v>1.2E-2</v>
+      </c>
+      <c r="H10" s="19">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="D11" s="34">
+        <v>1.4E-2</v>
+      </c>
+      <c r="H11" s="19">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="D12" s="34">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H12" s="19">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="D13" s="34">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H13" s="19">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="D14" s="34">
+        <v>0.02</v>
+      </c>
+      <c r="H14" s="19">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="D15" s="34">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H15" s="19">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="D16" s="34">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H16" s="19">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8">
+      <c r="D17" s="34">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="H17" s="19">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8">
+      <c r="D18" s="34">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="H18" s="19">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8">
+      <c r="D19" s="34">
+        <v>0.03</v>
+      </c>
+      <c r="H19" s="19">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8">
+      <c r="C21" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="34">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8">
+      <c r="D22" s="34">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8">
+      <c r="D23" s="34">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8">
+      <c r="D24" s="34">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8">
+      <c r="D25" s="34">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8">
+      <c r="D26" s="34">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8">
+      <c r="D27" s="34">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8">
+      <c r="D28" s="34">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8">
+      <c r="D29" s="34">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8">
+      <c r="D30" s="34">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8">
+      <c r="D31" s="34">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4">
+      <c r="C33" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="34">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4">
+      <c r="D34" s="34">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4">
+      <c r="D35" s="34">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4">
+      <c r="D36" s="34">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4">
+      <c r="D37" s="34">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4">
+      <c r="D38" s="34">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4">
+      <c r="D39" s="34">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4">
+      <c r="D40" s="34">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4">
+      <c r="D41" s="34">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4">
+      <c r="D42" s="34">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4">
+      <c r="D43" s="34">
+        <v>0.03</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="H7:J7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BA409B-F542-984C-90DD-63A5E341973F}">
   <dimension ref="B2:Y9"/>
   <sheetViews>
@@ -7889,7 +9725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33EDBDFB-84C9-0D42-9872-D0E4DAFE61DB}">
   <dimension ref="B1:K9"/>
   <sheetViews>
@@ -8110,7 +9946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E95DD15-E630-164A-9911-8F448DFCB0FA}">
   <dimension ref="B1:Q33"/>
   <sheetViews>
@@ -8562,1452 +10398,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB14C90-9A0C-E346-B9BD-40AE56D235C4}">
-  <dimension ref="B1:BH46"/>
-  <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T48" sqref="T48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="5" style="4" customWidth="1"/>
-    <col min="2" max="4" width="7.875" style="4"/>
-    <col min="5" max="5" width="7.875" style="7"/>
-    <col min="6" max="7" width="7.875" style="4"/>
-    <col min="8" max="12" width="3.625" style="10" customWidth="1"/>
-    <col min="13" max="13" width="5" style="4" customWidth="1"/>
-    <col min="14" max="19" width="7.875" style="4"/>
-    <col min="20" max="24" width="3.625" style="10" customWidth="1"/>
-    <col min="25" max="25" width="5" style="4" customWidth="1"/>
-    <col min="26" max="28" width="7.875" style="4"/>
-    <col min="29" max="29" width="7.875" style="7"/>
-    <col min="30" max="30" width="7.875" style="8"/>
-    <col min="31" max="31" width="7.875" style="4"/>
-    <col min="32" max="36" width="3.625" style="10" customWidth="1"/>
-    <col min="37" max="37" width="5" style="4" customWidth="1"/>
-    <col min="38" max="39" width="7.875" style="4"/>
-    <col min="40" max="40" width="7.875" style="12"/>
-    <col min="41" max="41" width="7.875" style="4"/>
-    <col min="42" max="42" width="7.875" style="8"/>
-    <col min="43" max="43" width="7.875" style="4"/>
-    <col min="44" max="48" width="3.625" style="10" customWidth="1"/>
-    <col min="49" max="49" width="5" style="4" customWidth="1"/>
-    <col min="50" max="53" width="7.875" style="4"/>
-    <col min="54" max="54" width="7.875" style="8"/>
-    <col min="55" max="55" width="7.875" style="4"/>
-    <col min="56" max="60" width="3.625" style="10" customWidth="1"/>
-    <col min="61" max="16384" width="7.875" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:55" ht="15" customHeight="1">
-      <c r="Z1" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="2:55" ht="15" customHeight="1">
-      <c r="B2" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="85" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="N2" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="84"/>
-      <c r="S2" s="84"/>
-      <c r="Z2" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA2" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB2" s="84"/>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="84"/>
-      <c r="AE2" s="84"/>
-      <c r="AL2" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM2" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="AN2" s="84"/>
-      <c r="AO2" s="84"/>
-      <c r="AP2" s="84"/>
-      <c r="AQ2" s="84"/>
-      <c r="AY2" s="86" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ2" s="86"/>
-      <c r="BA2" s="15"/>
-      <c r="BB2" s="15"/>
-      <c r="BC2" s="15"/>
-    </row>
-    <row r="3" spans="2:55" ht="15" customHeight="1">
-      <c r="B3" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="4">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4">
-        <v>20</v>
-      </c>
-      <c r="F3" s="4">
-        <v>25</v>
-      </c>
-      <c r="G3" s="4">
-        <v>30</v>
-      </c>
-      <c r="H3" s="10">
-        <v>10</v>
-      </c>
-      <c r="I3" s="10">
-        <v>15</v>
-      </c>
-      <c r="J3" s="10">
-        <v>20</v>
-      </c>
-      <c r="K3" s="10">
-        <v>25</v>
-      </c>
-      <c r="L3" s="10">
-        <v>30</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="4">
-        <v>10</v>
-      </c>
-      <c r="P3" s="4">
-        <v>15</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>20</v>
-      </c>
-      <c r="R3" s="4">
-        <v>25</v>
-      </c>
-      <c r="S3" s="4">
-        <v>30</v>
-      </c>
-      <c r="T3" s="10">
-        <v>10</v>
-      </c>
-      <c r="U3" s="10">
-        <v>15</v>
-      </c>
-      <c r="V3" s="10">
-        <v>20</v>
-      </c>
-      <c r="W3" s="10">
-        <v>25</v>
-      </c>
-      <c r="X3" s="10">
-        <v>30</v>
-      </c>
-      <c r="Z3" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA3" s="4">
-        <v>10</v>
-      </c>
-      <c r="AB3" s="4">
-        <v>15</v>
-      </c>
-      <c r="AC3" s="4">
-        <v>20</v>
-      </c>
-      <c r="AD3" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="AE3" s="4">
-        <v>30</v>
-      </c>
-      <c r="AF3" s="10">
-        <v>10</v>
-      </c>
-      <c r="AG3" s="10">
-        <v>15</v>
-      </c>
-      <c r="AH3" s="10">
-        <v>20</v>
-      </c>
-      <c r="AI3" s="10">
-        <v>25</v>
-      </c>
-      <c r="AJ3" s="10">
-        <v>30</v>
-      </c>
-      <c r="AL3" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="AM3" s="4">
-        <v>10</v>
-      </c>
-      <c r="AN3" s="4">
-        <v>15</v>
-      </c>
-      <c r="AO3" s="4">
-        <v>20</v>
-      </c>
-      <c r="AP3" s="4">
-        <v>25</v>
-      </c>
-      <c r="AQ3" s="4">
-        <v>30</v>
-      </c>
-      <c r="AR3" s="10">
-        <v>10</v>
-      </c>
-      <c r="AS3" s="10">
-        <v>15</v>
-      </c>
-      <c r="AT3" s="10">
-        <v>20</v>
-      </c>
-      <c r="AU3" s="10">
-        <v>25</v>
-      </c>
-      <c r="AV3" s="10">
-        <v>30</v>
-      </c>
-      <c r="AY3" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="AZ3" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="BB3" s="4"/>
-    </row>
-    <row r="4" spans="2:55" ht="15" customHeight="1">
-      <c r="B4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="7">
-        <v>635.9</v>
-      </c>
-      <c r="D4" s="7">
-        <v>631.04</v>
-      </c>
-      <c r="E4" s="7">
-        <v>626.12</v>
-      </c>
-      <c r="F4" s="7">
-        <v>621.14</v>
-      </c>
-      <c r="G4" s="7">
-        <v>616.11</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="12"/>
-      <c r="Z4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA4" s="7">
-        <v>17.149999999999999</v>
-      </c>
-      <c r="AC4" s="7">
-        <v>16.05</v>
-      </c>
-      <c r="AD4" s="63">
-        <f>0.5*(AC4+AE4)</f>
-        <v>15.495000000000001</v>
-      </c>
-      <c r="AE4" s="4">
-        <v>14.94</v>
-      </c>
-      <c r="AF4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM4" s="8"/>
-      <c r="AN4" s="8"/>
-      <c r="AO4" s="8"/>
-      <c r="AQ4" s="8"/>
-      <c r="AX4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AY4" s="4">
-        <v>143.5</v>
-      </c>
-      <c r="AZ4" s="18">
-        <f t="shared" ref="AZ4:AZ15" si="0">AY4-273.15</f>
-        <v>-129.64999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="2:55" ht="15" customHeight="1">
-      <c r="B5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="7">
-        <v>668.37</v>
-      </c>
-      <c r="D5" s="7">
-        <v>663.91</v>
-      </c>
-      <c r="E5" s="7">
-        <v>659.42</v>
-      </c>
-      <c r="F5" s="7">
-        <v>654.89</v>
-      </c>
-      <c r="G5" s="7">
-        <v>650.33000000000004</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="12">
-        <v>0.2949</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA5" s="7">
-        <v>19.420000000000002</v>
-      </c>
-      <c r="AC5" s="7">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="AD5" s="63">
-        <f t="shared" ref="AD5:AD15" si="1">0.5*(AC5+AE5)</f>
-        <v>17.89</v>
-      </c>
-      <c r="AE5" s="4">
-        <v>17.38</v>
-      </c>
-      <c r="AF5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM5" s="8"/>
-      <c r="AN5" s="8"/>
-      <c r="AO5" s="8"/>
-      <c r="AQ5" s="8"/>
-      <c r="AX5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AY5" s="4">
-        <v>177.8</v>
-      </c>
-      <c r="AZ5" s="18">
-        <f t="shared" si="0"/>
-        <v>-95.349999999999966</v>
-      </c>
-    </row>
-    <row r="6" spans="2:55" ht="15" customHeight="1">
-      <c r="B6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="7">
-        <v>692.4</v>
-      </c>
-      <c r="D6" s="7">
-        <v>688.2</v>
-      </c>
-      <c r="E6" s="7">
-        <v>683.99</v>
-      </c>
-      <c r="F6" s="7">
-        <v>679.75</v>
-      </c>
-      <c r="G6" s="7">
-        <v>675.49</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="12">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="W6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA6" s="7">
-        <v>21.12</v>
-      </c>
-      <c r="AC6" s="7">
-        <v>20.14</v>
-      </c>
-      <c r="AD6" s="63">
-        <f t="shared" si="1"/>
-        <v>19.655000000000001</v>
-      </c>
-      <c r="AE6" s="4">
-        <v>19.170000000000002</v>
-      </c>
-      <c r="AF6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM6" s="8"/>
-      <c r="AN6" s="8"/>
-      <c r="AO6" s="8"/>
-      <c r="AQ6" s="8"/>
-      <c r="AX6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AY6" s="4">
-        <v>182.6</v>
-      </c>
-      <c r="AZ6" s="18">
-        <f t="shared" si="0"/>
-        <v>-90.549999999999983</v>
-      </c>
-    </row>
-    <row r="7" spans="2:55" ht="15" customHeight="1">
-      <c r="B7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="N7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="12">
-        <v>0.50919999999999999</v>
-      </c>
-      <c r="W7" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA7" s="7">
-        <v>22.57</v>
-      </c>
-      <c r="AC7" s="7">
-        <v>21.62</v>
-      </c>
-      <c r="AD7" s="63">
-        <f t="shared" si="1"/>
-        <v>21.145000000000003</v>
-      </c>
-      <c r="AE7" s="4">
-        <v>20.67</v>
-      </c>
-      <c r="AF7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AM7" s="8"/>
-      <c r="AN7" s="8">
-        <v>1.988</v>
-      </c>
-      <c r="AO7" s="8">
-        <v>2.14</v>
-      </c>
-      <c r="AP7" s="8">
-        <v>2.3559999999999999</v>
-      </c>
-      <c r="AQ7" s="8">
-        <v>2.633</v>
-      </c>
-      <c r="AS7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AY7" s="4">
-        <v>216.4</v>
-      </c>
-      <c r="AZ7" s="18">
-        <f t="shared" si="0"/>
-        <v>-56.749999999999972</v>
-      </c>
-    </row>
-    <row r="8" spans="2:55" ht="15" customHeight="1">
-      <c r="B8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="N8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="12"/>
-      <c r="Z8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA8" s="7">
-        <v>23.79</v>
-      </c>
-      <c r="AC8" s="7">
-        <v>22.85</v>
-      </c>
-      <c r="AD8" s="63">
-        <f t="shared" si="1"/>
-        <v>22.385000000000002</v>
-      </c>
-      <c r="AE8" s="4">
-        <v>21.92</v>
-      </c>
-      <c r="AF8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM8" s="8"/>
-      <c r="AN8" s="8">
-        <v>1.5249999999999999</v>
-      </c>
-      <c r="AO8" s="8">
-        <v>1.6259999999999999</v>
-      </c>
-      <c r="AP8" s="8">
-        <v>1.772</v>
-      </c>
-      <c r="AQ8" s="8">
-        <v>1.9610000000000001</v>
-      </c>
-      <c r="AS8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AY8" s="4">
-        <v>219.7</v>
-      </c>
-      <c r="AZ8" s="18">
-        <f t="shared" si="0"/>
-        <v>-53.449999999999989</v>
-      </c>
-    </row>
-    <row r="9" spans="2:55" ht="15" customHeight="1">
-      <c r="B9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="N9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="12">
-        <v>0.8498</v>
-      </c>
-      <c r="W9" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA9" s="7">
-        <v>24.75</v>
-      </c>
-      <c r="AC9" s="7">
-        <v>23.83</v>
-      </c>
-      <c r="AD9" s="63">
-        <f t="shared" si="1"/>
-        <v>23.369999999999997</v>
-      </c>
-      <c r="AE9" s="4">
-        <v>22.91</v>
-      </c>
-      <c r="AF9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM9" s="8"/>
-      <c r="AN9" s="8">
-        <v>1.165</v>
-      </c>
-      <c r="AO9" s="8">
-        <v>1.268</v>
-      </c>
-      <c r="AP9" s="8">
-        <v>1.3859999999999999</v>
-      </c>
-      <c r="AQ9" s="8">
-        <v>1.5589999999999999</v>
-      </c>
-      <c r="AS9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AY9" s="4">
-        <v>243.5</v>
-      </c>
-      <c r="AZ9" s="18">
-        <f t="shared" si="0"/>
-        <v>-29.649999999999977</v>
-      </c>
-    </row>
-    <row r="10" spans="2:55" ht="15" customHeight="1">
-      <c r="B10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="N10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="12"/>
-      <c r="Z10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA10" s="7">
-        <v>25.56</v>
-      </c>
-      <c r="AC10" s="7">
-        <v>24.66</v>
-      </c>
-      <c r="AD10" s="63">
-        <f t="shared" si="1"/>
-        <v>24.21</v>
-      </c>
-      <c r="AE10" s="4">
-        <v>23.76</v>
-      </c>
-      <c r="AF10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AM10" s="8"/>
-      <c r="AN10" s="8">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="AO10" s="8">
-        <v>1.0089999999999999</v>
-      </c>
-      <c r="AP10" s="8">
-        <v>1.1120000000000001</v>
-      </c>
-      <c r="AQ10" s="8">
-        <v>1.248</v>
-      </c>
-      <c r="AS10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AY10" s="4">
-        <v>247.6</v>
-      </c>
-      <c r="AZ10" s="18">
-        <f t="shared" si="0"/>
-        <v>-25.549999999999983</v>
-      </c>
-    </row>
-    <row r="11" spans="2:55" ht="15" customHeight="1">
-      <c r="B11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="N11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="12">
-        <v>1.3585</v>
-      </c>
-      <c r="W11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA11" s="7">
-        <v>26.24</v>
-      </c>
-      <c r="AC11" s="7">
-        <v>25.35</v>
-      </c>
-      <c r="AD11" s="63">
-        <f t="shared" si="1"/>
-        <v>24.91</v>
-      </c>
-      <c r="AE11" s="4">
-        <v>24.47</v>
-      </c>
-      <c r="AF11" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH11" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ11" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM11" s="8"/>
-      <c r="AN11" s="8">
-        <v>0.70799999999999996</v>
-      </c>
-      <c r="AO11" s="8">
-        <v>0.78800000000000003</v>
-      </c>
-      <c r="AP11" s="8">
-        <v>0.871</v>
-      </c>
-      <c r="AQ11" s="8">
-        <v>0.996</v>
-      </c>
-      <c r="AS11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AY11" s="4">
-        <v>263.60000000000002</v>
-      </c>
-      <c r="AZ11" s="18">
-        <f t="shared" si="0"/>
-        <v>-9.5499999999999545</v>
-      </c>
-    </row>
-    <row r="12" spans="2:55" ht="15" customHeight="1">
-      <c r="B12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="N12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="12"/>
-      <c r="Z12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA12" s="7">
-        <v>26.86</v>
-      </c>
-      <c r="AC12" s="7">
-        <v>25.99</v>
-      </c>
-      <c r="AD12" s="63">
-        <f t="shared" si="1"/>
-        <v>25.549999999999997</v>
-      </c>
-      <c r="AE12" s="4">
-        <v>25.11</v>
-      </c>
-      <c r="AF12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM12" s="8"/>
-      <c r="AN12" s="8">
-        <v>0.56499999999999995</v>
-      </c>
-      <c r="AO12" s="8">
-        <v>0.64</v>
-      </c>
-      <c r="AP12" s="8">
-        <v>0.70699999999999996</v>
-      </c>
-      <c r="AQ12" s="8">
-        <v>0.80500000000000005</v>
-      </c>
-      <c r="AS12" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT12" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU12" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV12" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AY12" s="4">
-        <v>267.8</v>
-      </c>
-      <c r="AZ12" s="18">
-        <f t="shared" si="0"/>
-        <v>-5.3499999999999659</v>
-      </c>
-    </row>
-    <row r="13" spans="2:55" ht="15" customHeight="1">
-      <c r="B13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="N13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="12">
-        <v>2.0779999999999998</v>
-      </c>
-      <c r="W13" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA13" s="7">
-        <v>27.43</v>
-      </c>
-      <c r="AC13" s="7">
-        <v>26.56</v>
-      </c>
-      <c r="AD13" s="63">
-        <f t="shared" si="1"/>
-        <v>26.125</v>
-      </c>
-      <c r="AE13" s="4">
-        <v>25.69</v>
-      </c>
-      <c r="AF13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AM13" s="8"/>
-      <c r="AN13" s="8">
-        <v>0.443</v>
-      </c>
-      <c r="AO13" s="8">
-        <v>0.495</v>
-      </c>
-      <c r="AP13" s="8">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="AQ13" s="8">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="AS13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AY13" s="4">
-        <v>279</v>
-      </c>
-      <c r="AZ13" s="18">
-        <f t="shared" si="0"/>
-        <v>5.8500000000000227</v>
-      </c>
-    </row>
-    <row r="14" spans="2:55" ht="15" customHeight="1">
-      <c r="B14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="N14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q14" s="7"/>
-      <c r="Z14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC14" s="7">
-        <v>27.07</v>
-      </c>
-      <c r="AD14" s="63">
-        <f t="shared" si="1"/>
-        <v>26.64</v>
-      </c>
-      <c r="AE14" s="4">
-        <v>26.21</v>
-      </c>
-      <c r="AH14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM14" s="8"/>
-      <c r="AN14" s="8">
-        <v>0.35699999999999998</v>
-      </c>
-      <c r="AO14" s="8">
-        <v>0.40400000000000003</v>
-      </c>
-      <c r="AP14" s="8">
-        <v>0.46100000000000002</v>
-      </c>
-      <c r="AQ14" s="8">
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="AS14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AY14" s="4">
-        <v>283.10000000000002</v>
-      </c>
-      <c r="AZ14" s="18">
-        <f t="shared" si="0"/>
-        <v>9.9500000000000455</v>
-      </c>
-    </row>
-    <row r="15" spans="2:55" ht="15" customHeight="1">
-      <c r="B15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="N15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q15" s="7"/>
-      <c r="Z15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC15" s="7">
-        <v>27.47</v>
-      </c>
-      <c r="AD15" s="63">
-        <f t="shared" si="1"/>
-        <v>27.045000000000002</v>
-      </c>
-      <c r="AE15" s="4">
-        <v>26.62</v>
-      </c>
-      <c r="AH15" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ15" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM15" s="8"/>
-      <c r="AN15" s="16"/>
-      <c r="AO15" s="8">
-        <v>0.34100000000000003</v>
-      </c>
-      <c r="AP15" s="8">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="AQ15" s="8">
-        <v>0.44600000000000001</v>
-      </c>
-      <c r="AT15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AY15" s="4">
-        <v>291.10000000000002</v>
-      </c>
-      <c r="AZ15" s="18">
-        <f t="shared" si="0"/>
-        <v>17.950000000000045</v>
-      </c>
-    </row>
-    <row r="16" spans="2:55" ht="15" customHeight="1">
-      <c r="Q16" s="7"/>
-      <c r="AM16" s="8"/>
-      <c r="AN16" s="16"/>
-      <c r="AO16" s="8"/>
-      <c r="AQ16" s="8"/>
-    </row>
-    <row r="17" spans="2:43" ht="15" customHeight="1">
-      <c r="Q17" s="7"/>
-      <c r="AM17" s="8"/>
-      <c r="AN17" s="16"/>
-      <c r="AO17" s="8"/>
-      <c r="AQ17" s="8"/>
-    </row>
-    <row r="18" spans="2:43" ht="15" customHeight="1">
-      <c r="B18" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
-    </row>
-    <row r="19" spans="2:43" ht="15" customHeight="1">
-      <c r="B19" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="4">
-        <v>10</v>
-      </c>
-      <c r="D19" s="4">
-        <v>15</v>
-      </c>
-      <c r="E19" s="4">
-        <v>20</v>
-      </c>
-      <c r="F19" s="4">
-        <v>25</v>
-      </c>
-      <c r="G19" s="4">
-        <v>30</v>
-      </c>
-      <c r="H19" s="10">
-        <v>10</v>
-      </c>
-      <c r="I19" s="10">
-        <v>15</v>
-      </c>
-      <c r="J19" s="10">
-        <v>20</v>
-      </c>
-      <c r="K19" s="10">
-        <v>25</v>
-      </c>
-      <c r="L19" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="2:43" ht="15" customHeight="1">
-      <c r="B20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7">
-        <v>626.20000000000005</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="J20" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="2:43" ht="15" customHeight="1">
-      <c r="B21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="F21" s="7">
-        <v>660.6</v>
-      </c>
-      <c r="G21" s="7"/>
-      <c r="K21" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="2:43" ht="15" customHeight="1">
-      <c r="B22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="F22" s="7">
-        <v>679.5</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="K22" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="2:43" ht="15" customHeight="1">
-      <c r="B23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="F23" s="7">
-        <v>698.6</v>
-      </c>
-      <c r="G23" s="7"/>
-      <c r="K23" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="2:43" ht="15" customHeight="1">
-      <c r="B24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7">
-        <v>719.2</v>
-      </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="J24" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="2:43" ht="15" customHeight="1">
-      <c r="B25" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="F25" s="7">
-        <v>726.6</v>
-      </c>
-      <c r="G25" s="7"/>
-      <c r="K25" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="2:43" ht="15" customHeight="1">
-      <c r="B26" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7">
-        <v>740.2</v>
-      </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="J26" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="2:43" ht="15" customHeight="1">
-      <c r="B27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7">
-        <v>749.5</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="J27" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="2:43" ht="15" customHeight="1">
-      <c r="B28" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7">
-        <v>756.4</v>
-      </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="J28" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="2:43" ht="15" customHeight="1">
-      <c r="B29" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7">
-        <v>759.6</v>
-      </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="J29" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="2:43" ht="15" customHeight="1">
-      <c r="B30" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7">
-        <v>768.5</v>
-      </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="J30" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="2:43" ht="15" customHeight="1">
-      <c r="B31" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="F31" s="7">
-        <v>770.1</v>
-      </c>
-      <c r="G31" s="7"/>
-      <c r="K31" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="6:14" ht="15" customHeight="1">
-      <c r="F33" s="5"/>
-    </row>
-    <row r="46" spans="6:14" ht="15" customHeight="1">
-      <c r="N46" s="17"/>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="AY2:AZ2"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="AA2:AE2"/>
-    <mergeCell ref="AM2:AQ2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Sun9-6 C8 input files
</commit_message>
<xml_diff>
--- a/simulation_plans_results.xlsx
+++ b/simulation_plans_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Dropbox\Github_Dropbox\AlkaneStudy.Gromacs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028A75F5-F758-40C8-9F99-83CE0157445E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FCCD05-51E5-425A-A12D-F899509B68CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EF8A33E0-ACA8-D640-B463-6863C93E9688}"/>
   </bookViews>
@@ -4129,7 +4129,7 @@
   <dimension ref="B2:M57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="H2" sqref="H2:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -4400,7 +4400,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:13">

</xml_diff>

<commit_message>
Finalized Sun9-6 C8 annealing input files
</commit_message>
<xml_diff>
--- a/simulation_plans_results.xlsx
+++ b/simulation_plans_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Dropbox\Github_Dropbox\AlkaneStudy.Gromacs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FCCD05-51E5-425A-A12D-F899509B68CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7783D95-0E6F-44FB-80DD-E1DFB780B4F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EF8A33E0-ACA8-D640-B463-6863C93E9688}"/>
   </bookViews>
@@ -27,7 +27,6 @@
     <sheet name="Expr old" sheetId="4" state="hidden" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="281">
   <si>
     <t>Study</t>
   </si>
@@ -1027,6 +1026,12 @@
   <si>
     <t>Ref</t>
   </si>
+  <si>
+    <t>FlexWilliams4TL-UA-torsion_1024xC16_properties_298K_1bar</t>
+  </si>
+  <si>
+    <t>ORIG</t>
+  </si>
 </sst>
 </file>
 
@@ -1039,7 +1044,7 @@
     <numFmt numFmtId="167" formatCode="0.00000"/>
     <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1154,13 +1159,6 @@
     </font>
     <font>
       <vertAlign val="superscript"/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1341,7 +1339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1623,19 +1621,19 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1644,13 +1642,13 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1667,6 +1665,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1690,7 +1694,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1800,7 +1807,37 @@
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1851,37 +1888,37 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.15080993086311401</c:v>
+                  <c:v>2.5134988477185666E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10392223160637679</c:v>
+                  <c:v>1.7320371934396131E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.846090679015647E-2</c:v>
+                  <c:v>1.1410151131692746E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3899020788525177E-2</c:v>
+                  <c:v>1.0649836798087529E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6418088036741173E-2</c:v>
+                  <c:v>2.7363480061235288E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.4159613555745184E-2</c:v>
+                  <c:v>5.6932689259575307E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3377149515878035E-2</c:v>
+                  <c:v>3.8961915859796726E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.916235671942655E-2</c:v>
+                  <c:v>8.1937261199044251E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.3731112624836202E-2</c:v>
+                  <c:v>1.5621852104139368E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.10666187349319943</c:v>
+                  <c:v>1.7776978915533238E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.18810473179140902</c:v>
+                  <c:v>3.1350788631901501E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4129,7 +4166,7 @@
   <dimension ref="B2:M57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H15"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -4455,7 +4492,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:13" s="92" customFormat="1">
@@ -4623,6 +4660,9 @@
       <c r="G24" s="14" t="s">
         <v>188</v>
       </c>
+      <c r="J24" s="14" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="25" spans="2:10">
       <c r="C25" s="14" t="s">
@@ -4638,6 +4678,9 @@
       </c>
       <c r="C26" s="14" t="s">
         <v>180</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="2:10" s="92" customFormat="1">
@@ -5142,7 +5185,7 @@
   <dimension ref="B1:Q33"/>
   <sheetViews>
     <sheetView zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -5158,29 +5201,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17">
-      <c r="I1" s="121" t="s">
+      <c r="I1" s="123" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="123"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="123"/>
     </row>
     <row r="2" spans="2:17">
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="117" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="115"/>
+      <c r="D2" s="117"/>
       <c r="F2" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="I2" s="121" t="s">
+      <c r="I2" s="123" t="s">
         <v>120</v>
       </c>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
       <c r="L2" s="14" t="s">
         <v>121</v>
       </c>
@@ -5658,51 +5701,51 @@
       <c r="F4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="119" t="s">
+      <c r="H4" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="119"/>
-      <c r="J4" s="119"/>
-      <c r="K4" s="119"/>
-      <c r="L4" s="119"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="121"/>
+      <c r="K4" s="121"/>
+      <c r="L4" s="121"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
-      <c r="T4" s="119" t="s">
+      <c r="T4" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="119"/>
-      <c r="V4" s="119"/>
-      <c r="W4" s="119"/>
-      <c r="X4" s="119"/>
+      <c r="U4" s="121"/>
+      <c r="V4" s="121"/>
+      <c r="W4" s="121"/>
+      <c r="X4" s="121"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="7"/>
-      <c r="AF4" s="119" t="s">
+      <c r="AF4" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="AG4" s="119"/>
-      <c r="AH4" s="119"/>
-      <c r="AI4" s="119"/>
-      <c r="AJ4" s="119"/>
+      <c r="AG4" s="121"/>
+      <c r="AH4" s="121"/>
+      <c r="AI4" s="121"/>
+      <c r="AJ4" s="121"/>
       <c r="AN4" s="10"/>
       <c r="AP4" s="7"/>
-      <c r="AR4" s="119" t="s">
+      <c r="AR4" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="AS4" s="119"/>
-      <c r="AT4" s="119"/>
-      <c r="AU4" s="119"/>
-      <c r="AV4" s="119"/>
+      <c r="AS4" s="121"/>
+      <c r="AT4" s="121"/>
+      <c r="AU4" s="121"/>
+      <c r="AV4" s="121"/>
       <c r="BB4" s="7"/>
-      <c r="BD4" s="119" t="s">
+      <c r="BD4" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="BE4" s="119"/>
-      <c r="BF4" s="119"/>
-      <c r="BG4" s="119"/>
-      <c r="BH4" s="119"/>
+      <c r="BE4" s="121"/>
+      <c r="BF4" s="121"/>
+      <c r="BG4" s="121"/>
+      <c r="BH4" s="121"/>
     </row>
     <row r="5" spans="2:60" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="B5" s="12" t="s">
@@ -6947,20 +6990,20 @@
       <c r="K3" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="M3" s="115" t="s">
+      <c r="M3" s="117" t="s">
         <v>81</v>
       </c>
-      <c r="N3" s="115"/>
-      <c r="O3" s="115"/>
-      <c r="Q3" s="115" t="s">
+      <c r="N3" s="117"/>
+      <c r="O3" s="117"/>
+      <c r="Q3" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="R3" s="115"/>
-      <c r="S3" s="115"/>
-      <c r="T3" s="115"/>
-      <c r="U3" s="115"/>
-      <c r="V3" s="115"/>
-      <c r="W3" s="115"/>
+      <c r="R3" s="117"/>
+      <c r="S3" s="117"/>
+      <c r="T3" s="117"/>
+      <c r="U3" s="117"/>
+      <c r="V3" s="117"/>
+      <c r="W3" s="117"/>
     </row>
     <row r="4" spans="2:24" s="15" customFormat="1">
       <c r="B4" s="15" t="s">
@@ -7861,20 +7904,20 @@
       <c r="O3" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="Q3" s="115" t="s">
+      <c r="Q3" s="117" t="s">
         <v>81</v>
       </c>
-      <c r="R3" s="115"/>
-      <c r="S3" s="116"/>
-      <c r="U3" s="115" t="s">
+      <c r="R3" s="117"/>
+      <c r="S3" s="118"/>
+      <c r="U3" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="V3" s="115"/>
-      <c r="W3" s="115"/>
-      <c r="X3" s="115"/>
-      <c r="Y3" s="115"/>
-      <c r="Z3" s="115"/>
-      <c r="AA3" s="115"/>
+      <c r="V3" s="117"/>
+      <c r="W3" s="117"/>
+      <c r="X3" s="117"/>
+      <c r="Y3" s="117"/>
+      <c r="Z3" s="117"/>
+      <c r="AA3" s="117"/>
     </row>
     <row r="4" spans="2:28" s="15" customFormat="1">
       <c r="B4" s="15" t="s">
@@ -8287,10 +8330,10 @@
   <dimension ref="B2:AC50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J35" sqref="J35"/>
+      <selection pane="bottomRight" activeCell="AC22" sqref="AC22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -8330,20 +8373,20 @@
       <c r="Q3" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="S3" s="115" t="s">
+      <c r="S3" s="117" t="s">
         <v>81</v>
       </c>
-      <c r="T3" s="115"/>
-      <c r="U3" s="116"/>
-      <c r="W3" s="115" t="s">
+      <c r="T3" s="117"/>
+      <c r="U3" s="118"/>
+      <c r="W3" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="X3" s="115"/>
-      <c r="Y3" s="115"/>
-      <c r="Z3" s="115"/>
-      <c r="AA3" s="115"/>
-      <c r="AB3" s="115"/>
-      <c r="AC3" s="115"/>
+      <c r="X3" s="117"/>
+      <c r="Y3" s="117"/>
+      <c r="Z3" s="117"/>
+      <c r="AA3" s="117"/>
+      <c r="AB3" s="117"/>
+      <c r="AC3" s="117"/>
     </row>
     <row r="4" spans="2:29" s="15" customFormat="1">
       <c r="B4" s="15" t="s">
@@ -9153,6 +9196,9 @@
       <c r="AB21" s="74"/>
     </row>
     <row r="22" spans="2:29" s="71" customFormat="1">
+      <c r="B22" s="71" t="s">
+        <v>279</v>
+      </c>
       <c r="C22" s="71" t="s">
         <v>216</v>
       </c>
@@ -9563,10 +9609,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2C844C-ED1A-4540-A821-8B893B2A81D6}">
-  <dimension ref="B1:U43"/>
+  <dimension ref="B1:U46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -9680,19 +9726,19 @@
       </c>
     </row>
     <row r="7" spans="2:21">
-      <c r="C7" s="117" t="s">
+      <c r="C7" s="119" t="s">
         <v>243</v>
       </c>
-      <c r="D7" s="117"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
       <c r="H7" s="89"/>
-      <c r="L7" s="117" t="s">
+      <c r="L7" s="119" t="s">
         <v>244</v>
       </c>
-      <c r="M7" s="117"/>
-      <c r="N7" s="117"/>
+      <c r="M7" s="119"/>
+      <c r="N7" s="119"/>
     </row>
     <row r="8" spans="2:21" s="90" customFormat="1">
       <c r="D8" s="80" t="s">
@@ -9757,8 +9803,8 @@
         <v>8.3302353252099337E-2</v>
       </c>
       <c r="J9" s="114">
-        <f>I9+I21+I33</f>
-        <v>0.15080993086311401</v>
+        <f>(I9+I21+I33)/6</f>
+        <v>2.5134988477185666E-2</v>
       </c>
       <c r="L9" s="85">
         <v>1.4E-2</v>
@@ -9795,8 +9841,8 @@
         <v>5.9288271597642751E-2</v>
       </c>
       <c r="J10" s="114">
-        <f t="shared" ref="J10:J19" si="2">I10+I22+I34</f>
-        <v>0.10392223160637679</v>
+        <f t="shared" ref="J10:J19" si="2">(I10+I22+I34)/6</f>
+        <v>1.7320371934396131E-2</v>
       </c>
       <c r="L10" s="85">
         <v>1.4999999999999999E-2</v>
@@ -9834,7 +9880,7 @@
       </c>
       <c r="J11" s="114">
         <f t="shared" si="2"/>
-        <v>6.846090679015647E-2</v>
+        <v>1.1410151131692746E-2</v>
       </c>
       <c r="L11" s="85">
         <v>1.6E-2</v>
@@ -9872,7 +9918,7 @@
       </c>
       <c r="J12" s="114">
         <f t="shared" si="2"/>
-        <v>6.3899020788525177E-2</v>
+        <v>1.0649836798087529E-2</v>
       </c>
       <c r="L12" s="85">
         <v>1.7000000000000001E-2</v>
@@ -9910,7 +9956,7 @@
       </c>
       <c r="J13" s="114">
         <f t="shared" si="2"/>
-        <v>1.6418088036741173E-2</v>
+        <v>2.7363480061235288E-3</v>
       </c>
       <c r="L13" s="85">
         <v>1.7999999999999999E-2</v>
@@ -9925,41 +9971,41 @@
         <v>0.3322</v>
       </c>
     </row>
-    <row r="14" spans="2:21">
-      <c r="D14" s="84">
+    <row r="14" spans="2:21" s="124" customFormat="1">
+      <c r="D14" s="36">
         <v>0.02</v>
       </c>
-      <c r="E14" s="84">
+      <c r="E14" s="36">
         <v>7.9587500000000002</v>
       </c>
-      <c r="F14" s="88">
+      <c r="F14" s="124">
         <v>763.78099999999995</v>
       </c>
-      <c r="G14" s="87">
+      <c r="G14" s="39">
         <v>0.32100000000000001</v>
       </c>
-      <c r="H14" s="84">
+      <c r="H14" s="36">
         <f t="shared" si="0"/>
         <v>0.34331847401325505</v>
       </c>
-      <c r="I14" s="114">
+      <c r="I14" s="125">
         <f t="shared" si="1"/>
         <v>1.2807453588471695E-2</v>
       </c>
       <c r="J14" s="114">
         <f t="shared" si="2"/>
-        <v>3.4159613555745184E-2</v>
-      </c>
-      <c r="L14" s="85">
+        <v>5.6932689259575307E-3</v>
+      </c>
+      <c r="L14" s="124">
         <v>1.9E-2</v>
       </c>
-      <c r="S14" s="84">
+      <c r="S14" s="36">
         <v>7.9587500000000002</v>
       </c>
-      <c r="T14" s="85">
+      <c r="T14" s="124">
         <v>763.78099999999995</v>
       </c>
-      <c r="U14" s="87">
+      <c r="U14" s="39">
         <v>0.3241</v>
       </c>
     </row>
@@ -9986,7 +10032,7 @@
       </c>
       <c r="J15" s="114">
         <f t="shared" si="2"/>
-        <v>2.3377149515878035E-2</v>
+        <v>3.8961915859796726E-3</v>
       </c>
       <c r="L15" s="85">
         <v>0.02</v>
@@ -10024,7 +10070,7 @@
       </c>
       <c r="J16" s="114">
         <f t="shared" si="2"/>
-        <v>4.916235671942655E-2</v>
+        <v>8.1937261199044251E-3</v>
       </c>
       <c r="L16" s="85">
         <v>2.1000000000000001E-2</v>
@@ -10062,7 +10108,7 @@
       </c>
       <c r="J17" s="114">
         <f t="shared" si="2"/>
-        <v>9.3731112624836202E-2</v>
+        <v>1.5621852104139368E-2</v>
       </c>
       <c r="L17" s="85">
         <v>2.1999999999999999E-2</v>
@@ -10100,7 +10146,7 @@
       </c>
       <c r="J18" s="114">
         <f t="shared" si="2"/>
-        <v>0.10666187349319943</v>
+        <v>1.7776978915533238E-2</v>
       </c>
       <c r="L18" s="85">
         <v>2.3E-2</v>
@@ -10138,7 +10184,7 @@
       </c>
       <c r="J19" s="114">
         <f t="shared" si="2"/>
-        <v>0.18810473179140902</v>
+        <v>3.1350788631901501E-2</v>
       </c>
       <c r="L19" s="85">
         <v>2.4E-2</v>
@@ -10269,24 +10315,24 @@
         <v>2.7507353427601283E-3</v>
       </c>
     </row>
-    <row r="26" spans="3:21">
-      <c r="D26" s="84">
+    <row r="26" spans="3:21" s="124" customFormat="1">
+      <c r="D26" s="36">
         <v>0.02</v>
       </c>
-      <c r="E26" s="84">
+      <c r="E26" s="36">
         <v>7.8100699999999996</v>
       </c>
-      <c r="F26" s="88">
+      <c r="F26" s="124">
         <v>758.17200000000003</v>
       </c>
-      <c r="G26" s="87">
+      <c r="G26" s="39">
         <v>0.38090000000000002</v>
       </c>
-      <c r="H26" s="84">
+      <c r="H26" s="36">
         <f t="shared" si="3"/>
         <v>0.40863828884320291</v>
       </c>
-      <c r="I26" s="114">
+      <c r="I26" s="125">
         <f t="shared" si="4"/>
         <v>1.2980044410776503E-2</v>
       </c>
@@ -10517,24 +10563,24 @@
         <v>2.5050208716763923E-3</v>
       </c>
     </row>
-    <row r="38" spans="3:9">
-      <c r="D38" s="84">
+    <row r="38" spans="3:9" s="124" customFormat="1">
+      <c r="D38" s="36">
         <v>0.02</v>
       </c>
-      <c r="E38" s="84">
+      <c r="E38" s="36">
         <v>8.2729499999999998</v>
       </c>
-      <c r="F38" s="88">
+      <c r="F38" s="124">
         <v>686.07799999999997</v>
       </c>
-      <c r="G38" s="87">
+      <c r="G38" s="39">
         <v>2.4076</v>
       </c>
-      <c r="H38" s="84">
+      <c r="H38" s="36">
         <f t="shared" si="5"/>
         <v>2.5673954490450415</v>
       </c>
-      <c r="I38" s="114">
+      <c r="I38" s="125">
         <f t="shared" si="6"/>
         <v>8.3721155564969868E-3</v>
       </c>
@@ -10647,6 +10693,31 @@
       <c r="I43" s="114">
         <f t="shared" si="6"/>
         <v>0.11415500926748777</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9">
+      <c r="C46" s="85" t="s">
+        <v>280</v>
+      </c>
+      <c r="D46" s="84">
+        <v>0.01</v>
+      </c>
+      <c r="E46" s="84">
+        <v>7.8995300000000004</v>
+      </c>
+      <c r="F46" s="116">
+        <v>802</v>
+      </c>
+      <c r="G46" s="87">
+        <v>0.19</v>
+      </c>
+      <c r="H46" s="84">
+        <f>G46/(1-$I$3*F$3/E46)</f>
+        <v>0.20331628558821369</v>
+      </c>
+      <c r="I46" s="114">
+        <f>((F46-$G$3)/$G$3)^2 + ((H46-$D$3)/$D$3)^2</f>
+        <v>0.226994189013701</v>
       </c>
     </row>
   </sheetData>
@@ -10702,20 +10773,20 @@
       <c r="L3" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="N3" s="115" t="s">
+      <c r="N3" s="117" t="s">
         <v>81</v>
       </c>
-      <c r="O3" s="115"/>
-      <c r="P3" s="116"/>
-      <c r="R3" s="115" t="s">
+      <c r="O3" s="117"/>
+      <c r="P3" s="118"/>
+      <c r="R3" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="S3" s="115"/>
-      <c r="T3" s="115"/>
-      <c r="U3" s="115"/>
-      <c r="V3" s="115"/>
-      <c r="W3" s="115"/>
-      <c r="X3" s="115"/>
+      <c r="S3" s="117"/>
+      <c r="T3" s="117"/>
+      <c r="U3" s="117"/>
+      <c r="V3" s="117"/>
+      <c r="W3" s="117"/>
+      <c r="X3" s="117"/>
     </row>
     <row r="4" spans="2:25" s="15" customFormat="1">
       <c r="B4" s="15" t="s">
@@ -10977,8 +11048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB14C90-9A0C-E346-B9BD-40AE56D235C4}">
   <dimension ref="B1:BH45"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="BA4" sqref="BA4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R48" sqref="R48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="15" customHeight="1"/>
@@ -11039,30 +11110,30 @@
       <c r="B2" s="93" t="s">
         <v>259</v>
       </c>
-      <c r="C2" s="120" t="s">
+      <c r="C2" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="119" t="s">
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
       <c r="N2" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="120" t="s">
+      <c r="O2" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="120"/>
-      <c r="S2" s="120"/>
+      <c r="P2" s="122"/>
+      <c r="Q2" s="122"/>
+      <c r="R2" s="122"/>
+      <c r="S2" s="122"/>
       <c r="T2" s="76"/>
       <c r="U2" s="76"/>
       <c r="V2" s="76"/>
@@ -11071,13 +11142,13 @@
       <c r="Z2" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="120" t="s">
+      <c r="AA2" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="AB2" s="120"/>
-      <c r="AC2" s="120"/>
-      <c r="AD2" s="120"/>
-      <c r="AE2" s="120"/>
+      <c r="AB2" s="122"/>
+      <c r="AC2" s="122"/>
+      <c r="AD2" s="122"/>
+      <c r="AE2" s="122"/>
       <c r="AF2" s="76"/>
       <c r="AG2" s="76"/>
       <c r="AH2" s="76"/>
@@ -11086,13 +11157,13 @@
       <c r="AL2" s="84" t="s">
         <v>260</v>
       </c>
-      <c r="AM2" s="120" t="s">
+      <c r="AM2" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="AN2" s="120"/>
-      <c r="AO2" s="120"/>
-      <c r="AP2" s="120"/>
-      <c r="AQ2" s="120"/>
+      <c r="AN2" s="122"/>
+      <c r="AO2" s="122"/>
+      <c r="AP2" s="122"/>
+      <c r="AQ2" s="122"/>
       <c r="AR2" s="76"/>
       <c r="AS2" s="76"/>
       <c r="AT2" s="76"/>
@@ -11250,7 +11321,7 @@
       <c r="AZ3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="BA3" s="122" t="s">
+      <c r="BA3" s="115" t="s">
         <v>278</v>
       </c>
       <c r="BD3" s="76"/>
@@ -12232,33 +12303,33 @@
       <c r="B17" s="93" t="s">
         <v>259</v>
       </c>
-      <c r="C17" s="118" t="s">
+      <c r="C17" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="118"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
+      <c r="G17" s="120"/>
       <c r="N17" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="O17" s="118" t="s">
+      <c r="O17" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="P17" s="118"/>
-      <c r="Q17" s="118"/>
-      <c r="R17" s="118"/>
-      <c r="S17" s="118"/>
+      <c r="P17" s="120"/>
+      <c r="Q17" s="120"/>
+      <c r="R17" s="120"/>
+      <c r="S17" s="120"/>
       <c r="AL17" s="84" t="s">
         <v>260</v>
       </c>
-      <c r="AM17" s="120" t="s">
+      <c r="AM17" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="AN17" s="120"/>
-      <c r="AO17" s="120"/>
-      <c r="AP17" s="120"/>
-      <c r="AQ17" s="120"/>
+      <c r="AN17" s="122"/>
+      <c r="AO17" s="122"/>
+      <c r="AP17" s="122"/>
+      <c r="AQ17" s="122"/>
       <c r="AR17" s="76"/>
       <c r="AS17" s="76"/>
       <c r="AT17" s="76"/>
@@ -12879,40 +12950,40 @@
       <c r="B32" s="93" t="s">
         <v>259</v>
       </c>
-      <c r="C32" s="120" t="s">
+      <c r="C32" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="120"/>
-      <c r="E32" s="120"/>
-      <c r="F32" s="120"/>
-      <c r="G32" s="120"/>
-      <c r="H32" s="119" t="s">
+      <c r="D32" s="122"/>
+      <c r="E32" s="122"/>
+      <c r="F32" s="122"/>
+      <c r="G32" s="122"/>
+      <c r="H32" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="I32" s="119"/>
-      <c r="J32" s="119"/>
-      <c r="K32" s="119"/>
-      <c r="L32" s="119"/>
+      <c r="I32" s="121"/>
+      <c r="J32" s="121"/>
+      <c r="K32" s="121"/>
+      <c r="L32" s="121"/>
       <c r="N32" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="O32" s="118" t="s">
+      <c r="O32" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="P32" s="118"/>
-      <c r="Q32" s="118"/>
-      <c r="R32" s="118"/>
-      <c r="S32" s="118"/>
+      <c r="P32" s="120"/>
+      <c r="Q32" s="120"/>
+      <c r="R32" s="120"/>
+      <c r="S32" s="120"/>
       <c r="AL32" s="84" t="s">
         <v>260</v>
       </c>
-      <c r="AM32" s="120" t="s">
+      <c r="AM32" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="AN32" s="120"/>
-      <c r="AO32" s="120"/>
-      <c r="AP32" s="120"/>
-      <c r="AQ32" s="120"/>
+      <c r="AN32" s="122"/>
+      <c r="AO32" s="122"/>
+      <c r="AP32" s="122"/>
+      <c r="AQ32" s="122"/>
       <c r="AR32" s="76"/>
       <c r="AS32" s="76"/>
       <c r="AT32" s="76"/>

</xml_diff>

<commit_message>
Fixed T range in GPU-111, added GPU-112 and 113.
</commit_message>
<xml_diff>
--- a/simulation_plans_results.xlsx
+++ b/simulation_plans_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Dropbox\Github_Dropbox\AlkaneStudy.Gromacs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844C1BE8-3281-4434-8108-05D8EED0A70C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931579BA-072F-42D3-A40C-6509B79114D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="10" xr2:uid="{EF8A33E0-ACA8-D640-B463-6863C93E9688}"/>
+    <workbookView xWindow="345" yWindow="345" windowWidth="2400" windowHeight="585" activeTab="10" xr2:uid="{EF8A33E0-ACA8-D640-B463-6863C93E9688}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim matrix" sheetId="13" r:id="rId1"/>
@@ -23,14 +23,15 @@
     <sheet name="Williams7" sheetId="19" r:id="rId8"/>
     <sheet name="FlexWilliams_old" sheetId="10" r:id="rId9"/>
     <sheet name="WilliamsOpt" sheetId="14" r:id="rId10"/>
-    <sheet name="C16_cryst" sheetId="21" r:id="rId11"/>
-    <sheet name="Williams2019" sheetId="18" r:id="rId12"/>
-    <sheet name="GMX_dihedral" sheetId="15" r:id="rId13"/>
-    <sheet name="Expr data" sheetId="2" r:id="rId14"/>
-    <sheet name="Ref" sheetId="3" r:id="rId15"/>
-    <sheet name="box_sizes" sheetId="5" r:id="rId16"/>
-    <sheet name="cos-acc tests" sheetId="7" state="hidden" r:id="rId17"/>
-    <sheet name="Expr old" sheetId="4" state="hidden" r:id="rId18"/>
+    <sheet name="Unit cells" sheetId="22" r:id="rId11"/>
+    <sheet name="Super-cells" sheetId="21" r:id="rId12"/>
+    <sheet name="Williams2019" sheetId="18" r:id="rId13"/>
+    <sheet name="GMX_dihedral" sheetId="15" r:id="rId14"/>
+    <sheet name="Expr data" sheetId="2" r:id="rId15"/>
+    <sheet name="Ref" sheetId="3" r:id="rId16"/>
+    <sheet name="box_sizes" sheetId="5" r:id="rId17"/>
+    <sheet name="cos-acc tests" sheetId="7" state="hidden" r:id="rId18"/>
+    <sheet name="Expr old" sheetId="4" state="hidden" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2015" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2033" uniqueCount="454">
   <si>
     <t>Study</t>
   </si>
@@ -1466,9 +1467,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Triclinic unit cell</t>
-  </si>
-  <si>
     <t>na</t>
   </si>
   <si>
@@ -1527,9 +1525,6 @@
     <t>GPU-113_CHARMM36-CTL_1024xC8_anneal_260-160-260K_100ns</t>
   </si>
   <si>
-    <t>GPU-112</t>
-  </si>
-  <si>
     <t>GPU-111_CHARMM36-CTL_512xC16_anneal_340-240-340K_100ns</t>
   </si>
   <si>
@@ -1560,13 +1555,40 @@
     <t>β</t>
   </si>
   <si>
-    <t>SG</t>
-  </si>
-  <si>
     <t>Triclinic</t>
   </si>
   <si>
     <t>Orthorhombic</t>
+  </si>
+  <si>
+    <t>GPU-112_CHARMM36-CTL_512xC15_anneal_330-230-330K_100ns</t>
+  </si>
+  <si>
+    <t>P-1</t>
+  </si>
+  <si>
+    <t>Space group</t>
+  </si>
+  <si>
+    <t>QQQFBP01</t>
+  </si>
+  <si>
+    <t>QQQFBD</t>
+  </si>
+  <si>
+    <t>C16 Triclinic unit cell</t>
+  </si>
+  <si>
+    <t>QQQFBA</t>
+  </si>
+  <si>
+    <t>Pbcm</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Craig, J. MATER. CHEM., 1994, 4(6), 977-981</t>
   </si>
 </sst>
 </file>
@@ -1912,7 +1934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2508,28 +2530,22 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9423,8 +9439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E6099B-77F6-4CCD-9B30-DB7CF2E469C9}">
   <dimension ref="B1:M60"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -13940,207 +13956,424 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54734A79-229D-40A1-9EF2-2AA48E78AAE8}">
-  <dimension ref="B2:AE11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CE14D2-6A31-4EE7-987E-9C9B413F95A3}">
+  <dimension ref="B2:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="5.75" style="68" customWidth="1"/>
-    <col min="2" max="2" width="41.625" style="68" customWidth="1"/>
-    <col min="3" max="5" width="7.5" style="68" customWidth="1"/>
-    <col min="6" max="6" width="9" style="68"/>
-    <col min="7" max="15" width="9" style="71"/>
-    <col min="16" max="18" width="9" style="68"/>
-    <col min="19" max="19" width="3.25" style="68" customWidth="1"/>
-    <col min="20" max="20" width="9" style="211"/>
-    <col min="21" max="22" width="9" style="68"/>
-    <col min="23" max="24" width="17" style="68" customWidth="1"/>
-    <col min="25" max="16384" width="9" style="68"/>
+    <col min="1" max="1" width="7.125" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="17.25" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="12" max="12" width="47.625" style="186" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:31" s="187" customFormat="1">
+    <row r="2" spans="2:12">
+      <c r="B2" s="163"/>
+      <c r="C2" s="163" t="s">
+        <v>436</v>
+      </c>
+      <c r="D2" s="163" t="s">
+        <v>286</v>
+      </c>
+      <c r="E2" s="163" t="s">
+        <v>446</v>
+      </c>
+      <c r="F2" s="163" t="s">
+        <v>437</v>
+      </c>
+      <c r="G2" s="163" t="s">
+        <v>438</v>
+      </c>
+      <c r="H2" s="163" t="s">
+        <v>439</v>
+      </c>
+      <c r="I2" s="210" t="s">
+        <v>440</v>
+      </c>
+      <c r="J2" s="174" t="s">
+        <v>441</v>
+      </c>
+      <c r="K2" s="174" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="212" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" s="68" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>447</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>442</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>445</v>
+      </c>
+      <c r="F3" s="68">
+        <v>4.2698999999999998</v>
+      </c>
+      <c r="G3" s="68">
+        <v>4.8105000000000002</v>
+      </c>
+      <c r="H3" s="71">
+        <v>22.344999999999999</v>
+      </c>
+      <c r="I3" s="71">
+        <v>84.541200000000003</v>
+      </c>
+      <c r="J3" s="71">
+        <v>67.427800000000005</v>
+      </c>
+      <c r="K3" s="71">
+        <v>72.995900000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68" t="s">
+        <v>443</v>
+      </c>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>448</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>443</v>
+      </c>
+      <c r="E6" s="68" t="s">
+        <v>451</v>
+      </c>
+      <c r="F6" s="68">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="G6" s="68">
+        <v>7.29</v>
+      </c>
+      <c r="H6" s="68">
+        <v>36.590000000000003</v>
+      </c>
+      <c r="I6" s="68">
+        <v>90</v>
+      </c>
+      <c r="J6" s="68">
+        <v>90</v>
+      </c>
+      <c r="K6" s="68">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68" t="s">
+        <v>443</v>
+      </c>
+      <c r="E7" s="68" t="s">
+        <v>451</v>
+      </c>
+      <c r="F7" s="68">
+        <v>5.1040000000000001</v>
+      </c>
+      <c r="G7" s="68">
+        <v>7.5069999999999997</v>
+      </c>
+      <c r="H7" s="68">
+        <v>36.808</v>
+      </c>
+      <c r="I7" s="68">
+        <v>90</v>
+      </c>
+      <c r="J7" s="68">
+        <v>90</v>
+      </c>
+      <c r="K7" s="68">
+        <v>90</v>
+      </c>
+      <c r="L7" s="186" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="68" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>450</v>
+      </c>
+      <c r="D9" s="68" t="s">
+        <v>443</v>
+      </c>
+      <c r="E9" s="68" t="s">
+        <v>452</v>
+      </c>
+      <c r="F9" s="68">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="G9" s="68">
+        <v>7.22</v>
+      </c>
+      <c r="H9" s="68">
+        <v>31.53</v>
+      </c>
+      <c r="I9" s="68">
+        <v>90</v>
+      </c>
+      <c r="J9" s="68">
+        <v>90</v>
+      </c>
+      <c r="K9" s="68">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="68"/>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="68"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54734A79-229D-40A1-9EF2-2AA48E78AAE8}">
+  <dimension ref="B2:R11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="3.375" style="68" customWidth="1"/>
+    <col min="2" max="2" width="40.25" style="68" customWidth="1"/>
+    <col min="3" max="5" width="6.625" style="68" customWidth="1"/>
+    <col min="6" max="6" width="7.875" style="68" customWidth="1"/>
+    <col min="7" max="15" width="8" style="207" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="68"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" s="187" customFormat="1">
       <c r="C2" s="191" t="s">
         <v>414</v>
       </c>
       <c r="D2" s="191"/>
       <c r="E2" s="191"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
-      <c r="J2" s="160"/>
-      <c r="K2" s="160"/>
-      <c r="L2" s="160"/>
-      <c r="M2" s="160"/>
-      <c r="N2" s="160"/>
-      <c r="O2" s="160"/>
+      <c r="G2" s="166"/>
+      <c r="H2" s="166"/>
+      <c r="I2" s="166"/>
+      <c r="J2" s="166"/>
+      <c r="K2" s="166"/>
+      <c r="L2" s="166"/>
+      <c r="M2" s="166"/>
+      <c r="N2" s="166"/>
+      <c r="O2" s="166"/>
       <c r="Q2" s="187" t="s">
         <v>413</v>
       </c>
-      <c r="T2" s="212"/>
-    </row>
-    <row r="3" spans="2:31" s="163" customFormat="1">
+    </row>
+    <row r="3" spans="2:18" s="163" customFormat="1">
       <c r="B3" s="163" t="s">
         <v>415</v>
       </c>
       <c r="C3" s="163" t="s">
+        <v>416</v>
+      </c>
+      <c r="D3" s="163" t="s">
         <v>417</v>
       </c>
-      <c r="D3" s="163" t="s">
+      <c r="E3" s="163" t="s">
         <v>418</v>
       </c>
-      <c r="E3" s="163" t="s">
+      <c r="F3" s="163" t="s">
         <v>419</v>
       </c>
-      <c r="F3" s="163" t="s">
-        <v>420</v>
-      </c>
-      <c r="G3" s="174" t="s">
+      <c r="G3" s="165" t="s">
         <v>404</v>
       </c>
-      <c r="H3" s="174" t="s">
+      <c r="H3" s="165" t="s">
         <v>405</v>
       </c>
-      <c r="I3" s="174" t="s">
+      <c r="I3" s="165" t="s">
         <v>406</v>
       </c>
-      <c r="J3" s="174" t="s">
+      <c r="J3" s="165" t="s">
         <v>407</v>
       </c>
-      <c r="K3" s="174" t="s">
+      <c r="K3" s="165" t="s">
         <v>408</v>
       </c>
-      <c r="L3" s="174" t="s">
+      <c r="L3" s="165" t="s">
         <v>409</v>
       </c>
-      <c r="M3" s="174" t="s">
+      <c r="M3" s="165" t="s">
         <v>410</v>
       </c>
-      <c r="N3" s="174" t="s">
+      <c r="N3" s="165" t="s">
         <v>411</v>
       </c>
-      <c r="O3" s="174" t="s">
+      <c r="O3" s="165" t="s">
         <v>412</v>
       </c>
-      <c r="P3" s="207" t="s">
+      <c r="P3" s="208" t="s">
+        <v>424</v>
+      </c>
+      <c r="Q3" s="208" t="s">
         <v>425</v>
       </c>
-      <c r="Q3" s="207" t="s">
+      <c r="R3" s="208" t="s">
         <v>426</v>
       </c>
-      <c r="R3" s="207" t="s">
-        <v>427</v>
-      </c>
-      <c r="S3" s="207"/>
-      <c r="T3" s="213"/>
-      <c r="V3" s="163" t="s">
-        <v>438</v>
-      </c>
-      <c r="W3" s="163" t="s">
-        <v>286</v>
-      </c>
-      <c r="X3" s="163" t="s">
-        <v>444</v>
-      </c>
-      <c r="Y3" s="163" t="s">
-        <v>439</v>
-      </c>
-      <c r="Z3" s="163" t="s">
-        <v>440</v>
-      </c>
-      <c r="AA3" s="163" t="s">
-        <v>441</v>
-      </c>
-      <c r="AB3" s="210" t="s">
-        <v>442</v>
-      </c>
-      <c r="AC3" s="174" t="s">
-        <v>443</v>
-      </c>
-      <c r="AD3" s="174" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE3" s="174" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="4" spans="2:31" s="208" customFormat="1">
-      <c r="B4" s="208" t="s">
-        <v>416</v>
-      </c>
-      <c r="C4" s="208">
+    </row>
+    <row r="4" spans="2:18" s="209" customFormat="1">
+      <c r="B4" s="209" t="s">
+        <v>449</v>
+      </c>
+      <c r="C4" s="209">
         <v>1</v>
       </c>
-      <c r="D4" s="208">
+      <c r="D4" s="209">
         <v>1</v>
       </c>
-      <c r="E4" s="208">
+      <c r="E4" s="209">
         <v>1</v>
       </c>
-      <c r="F4" s="208">
+      <c r="F4" s="209">
         <f>C4*D4*E4</f>
         <v>1</v>
       </c>
-      <c r="G4" s="209">
+      <c r="G4" s="211">
         <v>0.42698999999999998</v>
       </c>
-      <c r="H4" s="209">
+      <c r="H4" s="211">
         <v>0.46002999999999999</v>
       </c>
-      <c r="I4" s="209">
+      <c r="I4" s="211">
         <v>2.06298</v>
       </c>
-      <c r="J4" s="209">
+      <c r="J4" s="211">
         <v>0</v>
       </c>
-      <c r="K4" s="209">
+      <c r="K4" s="211">
         <v>0</v>
       </c>
-      <c r="L4" s="209">
+      <c r="L4" s="211">
         <v>0.14065</v>
       </c>
-      <c r="M4" s="209">
+      <c r="M4" s="211">
         <v>0</v>
       </c>
-      <c r="N4" s="209">
+      <c r="N4" s="211">
         <v>0.85763</v>
       </c>
-      <c r="O4" s="209">
+      <c r="O4" s="211">
         <v>-3.9870000000000003E-2</v>
       </c>
-      <c r="P4" s="208" t="b">
+      <c r="P4" s="209" t="b">
         <f>IF(G4 &gt; 2*L4, TRUE)</f>
         <v>1</v>
       </c>
-      <c r="Q4" s="208" t="b">
+      <c r="Q4" s="209" t="b">
         <f>IF(G4 &gt; 2*N4, TRUE)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="208" t="b">
+      <c r="R4" s="209" t="b">
         <f>IF(H4 &gt; 2*O4,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="T4" s="214"/>
-      <c r="U4" s="68" t="s">
-        <v>42</v>
-      </c>
-      <c r="V4" s="68"/>
-      <c r="W4" s="68" t="s">
-        <v>445</v>
-      </c>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="68"/>
-      <c r="Z4" s="68"/>
-      <c r="AA4" s="71"/>
-      <c r="AB4" s="71"/>
-      <c r="AC4" s="71"/>
-      <c r="AD4" s="71"/>
-      <c r="AE4" s="71"/>
-    </row>
-    <row r="5" spans="2:31">
+    </row>
+    <row r="5" spans="2:18">
       <c r="C5" s="68">
         <v>4</v>
       </c>
@@ -14154,39 +14387,39 @@
         <f>C5*D5*E5</f>
         <v>16</v>
       </c>
-      <c r="G5" s="71">
+      <c r="G5" s="207">
         <f>C5*G$4</f>
         <v>1.7079599999999999</v>
       </c>
-      <c r="H5" s="71">
+      <c r="H5" s="207">
         <f>D5*H$4</f>
         <v>1.84012</v>
       </c>
-      <c r="I5" s="71">
+      <c r="I5" s="207">
         <f>E5*I$4</f>
         <v>2.06298</v>
       </c>
-      <c r="J5" s="71">
+      <c r="J5" s="207">
         <f>C5*J$4</f>
         <v>0</v>
       </c>
-      <c r="K5" s="71">
+      <c r="K5" s="207">
         <f>C5*K$4</f>
         <v>0</v>
       </c>
-      <c r="L5" s="71">
+      <c r="L5" s="207">
         <f>D5*L$4</f>
         <v>0.56259999999999999</v>
       </c>
-      <c r="M5" s="71">
+      <c r="M5" s="207">
         <f>D5*M$4</f>
         <v>0</v>
       </c>
-      <c r="N5" s="71">
+      <c r="N5" s="207">
         <f>E5*N$4</f>
         <v>0.85763</v>
       </c>
-      <c r="O5" s="71">
+      <c r="O5" s="207">
         <f>E5*O$4</f>
         <v>-3.9870000000000003E-2</v>
       </c>
@@ -14202,22 +14435,10 @@
         <f t="shared" ref="R5:R8" si="2">IF(H5 &gt; 2*O5,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="S5" s="187"/>
-      <c r="U5" s="68" t="s">
-        <v>41</v>
-      </c>
-      <c r="W5" s="68" t="s">
-        <v>446</v>
-      </c>
-      <c r="AA5" s="71"/>
-      <c r="AB5" s="71"/>
-      <c r="AC5" s="71"/>
-      <c r="AD5" s="71"/>
-      <c r="AE5" s="71"/>
-    </row>
-    <row r="6" spans="2:31">
+    </row>
+    <row r="6" spans="2:18">
       <c r="B6" s="68" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C6" s="68">
         <v>5</v>
@@ -14232,39 +14453,39 @@
         <f>C6*D6*E6</f>
         <v>25</v>
       </c>
-      <c r="G6" s="71">
+      <c r="G6" s="207">
         <f>C6*G$4</f>
         <v>2.1349499999999999</v>
       </c>
-      <c r="H6" s="71">
+      <c r="H6" s="207">
         <f>D6*H$4</f>
         <v>2.3001499999999999</v>
       </c>
-      <c r="I6" s="71">
+      <c r="I6" s="207">
         <f>E6*I$4</f>
         <v>2.06298</v>
       </c>
-      <c r="J6" s="71">
+      <c r="J6" s="207">
         <f>C6*J$4</f>
         <v>0</v>
       </c>
-      <c r="K6" s="71">
+      <c r="K6" s="207">
         <f>C6*K$4</f>
         <v>0</v>
       </c>
-      <c r="L6" s="71">
+      <c r="L6" s="207">
         <f>D6*L$4</f>
         <v>0.70324999999999993</v>
       </c>
-      <c r="M6" s="71">
+      <c r="M6" s="207">
         <f>D6*M$4</f>
         <v>0</v>
       </c>
-      <c r="N6" s="71">
+      <c r="N6" s="207">
         <f>E6*N$4</f>
         <v>0.85763</v>
       </c>
-      <c r="O6" s="71">
+      <c r="O6" s="207">
         <f>E6*O$4</f>
         <v>-3.9870000000000003E-2</v>
       </c>
@@ -14280,19 +14501,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="S6" s="187"/>
-      <c r="U6" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA6" s="71"/>
-      <c r="AB6" s="71"/>
-      <c r="AC6" s="71"/>
-      <c r="AD6" s="71"/>
-      <c r="AE6" s="71"/>
-    </row>
-    <row r="7" spans="2:31">
+    </row>
+    <row r="7" spans="2:18">
       <c r="B7" s="68" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C7" s="68">
         <f>2*C6</f>
@@ -14310,39 +14522,39 @@
         <f>C7*D7*E7</f>
         <v>200</v>
       </c>
-      <c r="G7" s="71">
+      <c r="G7" s="207">
         <f>C7*G$4</f>
         <v>4.2698999999999998</v>
       </c>
-      <c r="H7" s="71">
+      <c r="H7" s="207">
         <f>D7*H$4</f>
         <v>4.6002999999999998</v>
       </c>
-      <c r="I7" s="71">
+      <c r="I7" s="207">
         <f>E7*I$4</f>
         <v>4.1259600000000001</v>
       </c>
-      <c r="J7" s="71">
+      <c r="J7" s="207">
         <f>C7*J$4</f>
         <v>0</v>
       </c>
-      <c r="K7" s="71">
+      <c r="K7" s="207">
         <f>C7*K$4</f>
         <v>0</v>
       </c>
-      <c r="L7" s="71">
+      <c r="L7" s="207">
         <f>D7*L$4</f>
         <v>1.4064999999999999</v>
       </c>
-      <c r="M7" s="71">
+      <c r="M7" s="207">
         <f>D7*M$4</f>
         <v>0</v>
       </c>
-      <c r="N7" s="71">
+      <c r="N7" s="207">
         <f>E7*N$4</f>
         <v>1.71526</v>
       </c>
-      <c r="O7" s="71">
+      <c r="O7" s="207">
         <f>E7*O$4</f>
         <v>-7.9740000000000005E-2</v>
       </c>
@@ -14358,11 +14570,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="S7" s="187"/>
-    </row>
-    <row r="8" spans="2:31">
+    </row>
+    <row r="8" spans="2:18">
       <c r="B8" s="68" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C8" s="68">
         <f>3*C6</f>
@@ -14380,39 +14591,39 @@
         <f>C8*D8*E8</f>
         <v>675</v>
       </c>
-      <c r="G8" s="71">
+      <c r="G8" s="207">
         <f>C8*G$4</f>
         <v>6.4048499999999997</v>
       </c>
-      <c r="H8" s="71">
+      <c r="H8" s="207">
         <f>D8*H$4</f>
         <v>6.9004500000000002</v>
       </c>
-      <c r="I8" s="71">
+      <c r="I8" s="207">
         <f>E8*I$4</f>
         <v>6.1889400000000006</v>
       </c>
-      <c r="J8" s="71">
+      <c r="J8" s="207">
         <f>C8*J$4</f>
         <v>0</v>
       </c>
-      <c r="K8" s="71">
+      <c r="K8" s="207">
         <f>C8*K$4</f>
         <v>0</v>
       </c>
-      <c r="L8" s="71">
+      <c r="L8" s="207">
         <f>D8*L$4</f>
         <v>2.10975</v>
       </c>
-      <c r="M8" s="71">
+      <c r="M8" s="207">
         <f>D8*M$4</f>
         <v>0</v>
       </c>
-      <c r="N8" s="71">
+      <c r="N8" s="207">
         <f>E8*N$4</f>
         <v>2.5728900000000001</v>
       </c>
-      <c r="O8" s="71">
+      <c r="O8" s="207">
         <f>E8*O$4</f>
         <v>-0.11961000000000001</v>
       </c>
@@ -14428,11 +14639,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="S8" s="187"/>
-    </row>
-    <row r="9" spans="2:31">
+    </row>
+    <row r="9" spans="2:18">
       <c r="B9" s="68" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C9" s="68">
         <f>4*C6</f>
@@ -14450,39 +14660,39 @@
         <f>C9*D9*E9</f>
         <v>1600</v>
       </c>
-      <c r="G9" s="71">
+      <c r="G9" s="207">
         <f>C9*G$4</f>
         <v>8.5397999999999996</v>
       </c>
-      <c r="H9" s="71">
+      <c r="H9" s="207">
         <f>D9*H$4</f>
         <v>9.2005999999999997</v>
       </c>
-      <c r="I9" s="71">
+      <c r="I9" s="207">
         <f>E9*I$4</f>
         <v>8.2519200000000001</v>
       </c>
-      <c r="J9" s="71">
+      <c r="J9" s="207">
         <f>C9*J$4</f>
         <v>0</v>
       </c>
-      <c r="K9" s="71">
+      <c r="K9" s="207">
         <f>C9*K$4</f>
         <v>0</v>
       </c>
-      <c r="L9" s="71">
+      <c r="L9" s="207">
         <f>D9*L$4</f>
         <v>2.8129999999999997</v>
       </c>
-      <c r="M9" s="71">
+      <c r="M9" s="207">
         <f>D9*M$4</f>
         <v>0</v>
       </c>
-      <c r="N9" s="71">
+      <c r="N9" s="207">
         <f>E9*N$4</f>
         <v>3.43052</v>
       </c>
-      <c r="O9" s="71">
+      <c r="O9" s="207">
         <f>E9*O$4</f>
         <v>-0.15948000000000001</v>
       </c>
@@ -14498,11 +14708,10 @@
         <f>IF(H9 &gt; 2*O9,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="S9" s="187"/>
-    </row>
-    <row r="10" spans="2:31">
+    </row>
+    <row r="10" spans="2:18">
       <c r="B10" s="68" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C10" s="68">
         <v>16</v>
@@ -14517,39 +14726,39 @@
         <f>C10*D10*E10</f>
         <v>768</v>
       </c>
-      <c r="G10" s="71">
+      <c r="G10" s="207">
         <f>C10*G$4</f>
         <v>6.8318399999999997</v>
       </c>
-      <c r="H10" s="71">
+      <c r="H10" s="207">
         <f>D10*H$4</f>
         <v>7.3604799999999999</v>
       </c>
-      <c r="I10" s="71">
+      <c r="I10" s="207">
         <f>E10*I$4</f>
         <v>6.1889400000000006</v>
       </c>
-      <c r="J10" s="71">
+      <c r="J10" s="207">
         <f>C10*J$4</f>
         <v>0</v>
       </c>
-      <c r="K10" s="71">
+      <c r="K10" s="207">
         <f>C10*K$4</f>
         <v>0</v>
       </c>
-      <c r="L10" s="71">
+      <c r="L10" s="207">
         <f>D10*L$4</f>
         <v>2.2504</v>
       </c>
-      <c r="M10" s="71">
+      <c r="M10" s="207">
         <f>D10*M$4</f>
         <v>0</v>
       </c>
-      <c r="N10" s="71">
+      <c r="N10" s="207">
         <f>E10*N$4</f>
         <v>2.5728900000000001</v>
       </c>
-      <c r="O10" s="71">
+      <c r="O10" s="207">
         <f>E10*O$4</f>
         <v>-0.11961000000000001</v>
       </c>
@@ -14565,9 +14774,8 @@
         <f>IF(H10 &gt; 2*O10,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="S10" s="187"/>
-    </row>
-    <row r="11" spans="2:31">
+    </row>
+    <row r="11" spans="2:18">
       <c r="C11" s="68">
         <v>18</v>
       </c>
@@ -14581,39 +14789,39 @@
         <f>C11*D11*E11</f>
         <v>1296</v>
       </c>
-      <c r="G11" s="71">
+      <c r="G11" s="207">
         <f>C11*G$4</f>
         <v>7.6858199999999997</v>
       </c>
-      <c r="H11" s="71">
+      <c r="H11" s="207">
         <f>D11*H$4</f>
         <v>8.2805400000000002</v>
       </c>
-      <c r="I11" s="71">
+      <c r="I11" s="207">
         <f>E11*I$4</f>
         <v>8.2519200000000001</v>
       </c>
-      <c r="J11" s="71">
+      <c r="J11" s="207">
         <f>C11*J$4</f>
         <v>0</v>
       </c>
-      <c r="K11" s="71">
+      <c r="K11" s="207">
         <f>C11*K$4</f>
         <v>0</v>
       </c>
-      <c r="L11" s="71">
+      <c r="L11" s="207">
         <f>D11*L$4</f>
         <v>2.5316999999999998</v>
       </c>
-      <c r="M11" s="71">
+      <c r="M11" s="207">
         <f>D11*M$4</f>
         <v>0</v>
       </c>
-      <c r="N11" s="71">
+      <c r="N11" s="207">
         <f>E11*N$4</f>
         <v>3.43052</v>
       </c>
-      <c r="O11" s="71">
+      <c r="O11" s="207">
         <f>E11*O$4</f>
         <v>-0.15948000000000001</v>
       </c>
@@ -14629,13 +14837,12 @@
         <f>IF(H11 &gt; 2*O11,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="S11" s="187"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:E2"/>
   </mergeCells>
-  <conditionalFormatting sqref="P4:S11">
+  <conditionalFormatting sqref="P4:R11">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -14645,7 +14852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE901DC-C123-4CCA-841E-6DF30D04B418}">
   <dimension ref="B1:AA35"/>
   <sheetViews>
@@ -15351,7 +15558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFF03F4-0D0E-4240-A36F-5BB31F518425}">
   <dimension ref="B2:E61"/>
   <sheetViews>
@@ -16226,7 +16433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB14C90-9A0C-E346-B9BD-40AE56D235C4}">
   <dimension ref="B1:BH45"/>
   <sheetViews>
@@ -18741,7 +18948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BDCE98-34D0-4ABF-8516-E6ECC928D09D}">
   <dimension ref="B2:D32"/>
   <sheetViews>
@@ -18976,7 +19183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33EDBDFB-84C9-0D42-9872-D0E4DAFE61DB}">
   <dimension ref="B1:K10"/>
   <sheetViews>
@@ -19233,7 +19440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E95DD15-E630-164A-9911-8F448DFCB0FA}">
   <dimension ref="B1:Q33"/>
   <sheetViews>
@@ -19687,7 +19894,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C044A9FB-F8D3-4917-BFAB-FBE43DD433AF}">
   <dimension ref="B3:BH17"/>
   <sheetViews>
@@ -22576,7 +22783,7 @@
   <dimension ref="B2:W69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -24243,7 +24450,7 @@
   <dimension ref="B2:W34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -24614,7 +24821,7 @@
     </row>
     <row r="15" spans="2:23">
       <c r="B15" s="69" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C15" s="155" t="s">
         <v>42</v>
@@ -24648,7 +24855,7 @@
         <v>92</v>
       </c>
       <c r="P15" s="70" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="Q15" s="155" t="s">
         <v>304</v>
@@ -24818,7 +25025,7 @@
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="69" t="s">
-        <v>433</v>
+        <v>444</v>
       </c>
       <c r="C23" s="184" t="s">
         <v>41</v>
@@ -25019,7 +25226,7 @@
     </row>
     <row r="31" spans="2:19" s="187" customFormat="1">
       <c r="B31" s="69" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C31" s="187" t="s">
         <v>33</v>
@@ -25047,13 +25254,13 @@
         <v>100000000</v>
       </c>
       <c r="N31" s="188" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="O31" s="186" t="s">
         <v>92</v>
       </c>
       <c r="P31" s="70" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="S31" s="166"/>
     </row>
@@ -25066,7 +25273,7 @@
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="69" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C33" s="184" t="s">
         <v>33</v>
@@ -27039,7 +27246,7 @@
         <v>92</v>
       </c>
       <c r="P28" s="42" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="V28" s="141"/>
       <c r="X28" s="141"/>
@@ -27251,7 +27458,7 @@
         <v>92</v>
       </c>
       <c r="P38" s="42" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="41" spans="2:27" s="15" customFormat="1">

</xml_diff>

<commit_message>
Updated method for first Sun9-6 mixedphase
</commit_message>
<xml_diff>
--- a/simulation_plans_results.xlsx
+++ b/simulation_plans_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Dropbox\Github_Dropbox\AlkaneStudy.Gromacs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFCBAF3-AA0E-497C-BDC4-85AA3A84BFDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C9918B-256D-48AC-89A3-B893FC84C81D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="646" firstSheet="1" activeTab="13" xr2:uid="{EF8A33E0-ACA8-D640-B463-6863C93E9688}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="646" firstSheet="11" activeTab="11" xr2:uid="{EF8A33E0-ACA8-D640-B463-6863C93E9688}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim matrix" sheetId="13" r:id="rId1"/>
@@ -24,15 +24,16 @@
     <sheet name="FlexWilliams_old" sheetId="10" state="hidden" r:id="rId9"/>
     <sheet name="WilliamsOpt" sheetId="14" r:id="rId10"/>
     <sheet name="Williams2019" sheetId="18" r:id="rId11"/>
-    <sheet name="Unit cells" sheetId="22" r:id="rId12"/>
-    <sheet name="Super-cells" sheetId="21" r:id="rId13"/>
-    <sheet name="Crystal sims" sheetId="23" r:id="rId14"/>
-    <sheet name="GMX_dihedral" sheetId="15" r:id="rId15"/>
-    <sheet name="Expr data" sheetId="2" r:id="rId16"/>
-    <sheet name="Ref" sheetId="3" r:id="rId17"/>
-    <sheet name="box_sizes" sheetId="5" r:id="rId18"/>
-    <sheet name="cos-acc tests" sheetId="7" r:id="rId19"/>
-    <sheet name="Expr old" sheetId="4" state="hidden" r:id="rId20"/>
+    <sheet name="MixedPhase" sheetId="24" r:id="rId12"/>
+    <sheet name="Unit cells" sheetId="22" r:id="rId13"/>
+    <sheet name="Super-cells" sheetId="21" r:id="rId14"/>
+    <sheet name="Crystal sims" sheetId="23" r:id="rId15"/>
+    <sheet name="GMX_dihedral" sheetId="15" r:id="rId16"/>
+    <sheet name="Expr data" sheetId="2" r:id="rId17"/>
+    <sheet name="Ref" sheetId="3" r:id="rId18"/>
+    <sheet name="box_sizes" sheetId="5" r:id="rId19"/>
+    <sheet name="cos-acc tests" sheetId="7" r:id="rId20"/>
+    <sheet name="Expr old" sheetId="4" state="hidden" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="541">
   <si>
     <t>Study</t>
   </si>
@@ -1848,6 +1849,39 @@
   </si>
   <si>
     <t>283 fixed</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Melted</t>
+  </si>
+  <si>
+    <t>Decreased</t>
+  </si>
+  <si>
+    <t>Increased</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Underdermined (barely changed)</t>
+  </si>
+  <si>
+    <t>Froze</t>
+  </si>
+  <si>
+    <t>1.2nm cut</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>Molecule</t>
   </si>
 </sst>
 </file>
@@ -2236,7 +2270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="292">
+  <cellXfs count="293">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3025,6 +3059,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3065,18 +3114,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -11903,11 +11940,11 @@
       <c r="AH1" s="204"/>
     </row>
     <row r="2" spans="2:36">
-      <c r="B2" s="279" t="s">
+      <c r="B2" s="286" t="s">
         <v>305</v>
       </c>
-      <c r="C2" s="279"/>
-      <c r="D2" s="279"/>
+      <c r="C2" s="286"/>
+      <c r="D2" s="286"/>
       <c r="AC2" s="211"/>
       <c r="AD2" s="224"/>
       <c r="AE2" s="212"/>
@@ -12128,18 +12165,18 @@
       <c r="E15" s="77"/>
       <c r="G15" s="78"/>
       <c r="H15" s="77"/>
-      <c r="L15" s="278" t="s">
+      <c r="L15" s="285" t="s">
         <v>465</v>
       </c>
-      <c r="M15" s="278"/>
-      <c r="N15" s="278"/>
-      <c r="O15" s="278"/>
-      <c r="P15" s="278"/>
-      <c r="Q15" s="278"/>
-      <c r="R15" s="278"/>
-      <c r="S15" s="278"/>
-      <c r="T15" s="278"/>
-      <c r="U15" s="278"/>
+      <c r="M15" s="285"/>
+      <c r="N15" s="285"/>
+      <c r="O15" s="285"/>
+      <c r="P15" s="285"/>
+      <c r="Q15" s="285"/>
+      <c r="R15" s="285"/>
+      <c r="S15" s="285"/>
+      <c r="T15" s="285"/>
+      <c r="U15" s="285"/>
       <c r="V15" s="77"/>
       <c r="W15" s="114"/>
       <c r="X15" s="77"/>
@@ -12156,48 +12193,48 @@
       <c r="AJ15" s="205"/>
     </row>
     <row r="16" spans="2:36">
-      <c r="C16" s="279" t="s">
+      <c r="C16" s="286" t="s">
         <v>231</v>
       </c>
-      <c r="D16" s="279"/>
-      <c r="E16" s="279"/>
-      <c r="F16" s="279"/>
-      <c r="G16" s="279"/>
-      <c r="H16" s="279"/>
-      <c r="I16" s="279"/>
-      <c r="J16" s="279"/>
+      <c r="D16" s="286"/>
+      <c r="E16" s="286"/>
+      <c r="F16" s="286"/>
+      <c r="G16" s="286"/>
+      <c r="H16" s="286"/>
+      <c r="I16" s="286"/>
+      <c r="J16" s="286"/>
       <c r="K16" s="148"/>
       <c r="L16" s="172"/>
-      <c r="M16" s="280">
+      <c r="M16" s="287">
         <v>1</v>
       </c>
-      <c r="N16" s="280"/>
-      <c r="O16" s="280"/>
-      <c r="P16" s="280">
+      <c r="N16" s="287"/>
+      <c r="O16" s="287"/>
+      <c r="P16" s="287">
         <v>2</v>
       </c>
-      <c r="Q16" s="280"/>
-      <c r="R16" s="280"/>
-      <c r="S16" s="280">
+      <c r="Q16" s="287"/>
+      <c r="R16" s="287"/>
+      <c r="S16" s="287">
         <v>3</v>
       </c>
-      <c r="T16" s="280"/>
-      <c r="U16" s="280"/>
-      <c r="V16" s="280">
+      <c r="T16" s="287"/>
+      <c r="U16" s="287"/>
+      <c r="V16" s="287">
         <v>4</v>
       </c>
-      <c r="W16" s="280"/>
-      <c r="X16" s="280"/>
-      <c r="Y16" s="280">
+      <c r="W16" s="287"/>
+      <c r="X16" s="287"/>
+      <c r="Y16" s="287">
         <v>5</v>
       </c>
-      <c r="Z16" s="280"/>
-      <c r="AA16" s="281"/>
-      <c r="AB16" s="275" t="s">
+      <c r="Z16" s="287"/>
+      <c r="AA16" s="288"/>
+      <c r="AB16" s="282" t="s">
         <v>278</v>
       </c>
-      <c r="AC16" s="276"/>
-      <c r="AD16" s="277"/>
+      <c r="AC16" s="283"/>
+      <c r="AD16" s="284"/>
     </row>
     <row r="17" spans="2:46" s="79" customFormat="1">
       <c r="D17" s="75" t="s">
@@ -16917,23 +16954,23 @@
     <row r="4" spans="2:27">
       <c r="E4" s="146"/>
       <c r="F4" s="146"/>
-      <c r="J4" s="273" t="s">
+      <c r="J4" s="280" t="s">
         <v>289</v>
       </c>
-      <c r="K4" s="273"/>
-      <c r="N4" s="273" t="s">
+      <c r="K4" s="280"/>
+      <c r="N4" s="280" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="273"/>
-      <c r="Q4" s="273" t="s">
+      <c r="O4" s="280"/>
+      <c r="Q4" s="280" t="s">
         <v>99</v>
       </c>
-      <c r="R4" s="273"/>
-      <c r="S4" s="273"/>
-      <c r="T4" s="273"/>
-      <c r="U4" s="273"/>
-      <c r="V4" s="273"/>
-      <c r="W4" s="273"/>
+      <c r="R4" s="280"/>
+      <c r="S4" s="280"/>
+      <c r="T4" s="280"/>
+      <c r="U4" s="280"/>
+      <c r="V4" s="280"/>
+      <c r="W4" s="280"/>
       <c r="X4" s="146"/>
       <c r="AA4" s="146"/>
     </row>
@@ -17558,6 +17595,170 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3949D05-7376-4059-B96D-BFD0734F58BD}">
+  <dimension ref="B2:AA7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="5" max="24" width="5" style="271" customWidth="1"/>
+    <col min="27" max="30" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:27" s="56" customFormat="1">
+      <c r="B2" s="56" t="s">
+        <v>540</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>539</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="15">
+        <v>280</v>
+      </c>
+      <c r="F2" s="15">
+        <v>282</v>
+      </c>
+      <c r="G2" s="15">
+        <v>284</v>
+      </c>
+      <c r="H2" s="15">
+        <v>286</v>
+      </c>
+      <c r="I2" s="15">
+        <v>288</v>
+      </c>
+      <c r="J2" s="15">
+        <v>290</v>
+      </c>
+      <c r="K2" s="15">
+        <v>292</v>
+      </c>
+      <c r="L2" s="15">
+        <v>294</v>
+      </c>
+      <c r="M2" s="15">
+        <v>296</v>
+      </c>
+      <c r="N2" s="15">
+        <v>298</v>
+      </c>
+      <c r="O2" s="15">
+        <v>300</v>
+      </c>
+      <c r="P2" s="15">
+        <v>302</v>
+      </c>
+      <c r="Q2" s="15">
+        <v>304</v>
+      </c>
+      <c r="R2" s="15">
+        <v>306</v>
+      </c>
+      <c r="S2" s="15">
+        <v>308</v>
+      </c>
+      <c r="T2" s="15">
+        <v>310</v>
+      </c>
+      <c r="U2" s="15">
+        <v>312</v>
+      </c>
+      <c r="V2" s="15">
+        <v>314</v>
+      </c>
+      <c r="W2" s="15">
+        <v>316</v>
+      </c>
+      <c r="X2" s="15">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="2:27">
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
+        <v>538</v>
+      </c>
+      <c r="O3" s="271" t="s">
+        <v>530</v>
+      </c>
+      <c r="P3" s="271" t="s">
+        <v>470</v>
+      </c>
+      <c r="Q3" s="271" t="s">
+        <v>470</v>
+      </c>
+      <c r="R3" s="271" t="s">
+        <v>531</v>
+      </c>
+      <c r="S3" s="271" t="s">
+        <v>470</v>
+      </c>
+      <c r="T3" s="271" t="s">
+        <v>470</v>
+      </c>
+      <c r="U3" s="271" t="s">
+        <v>62</v>
+      </c>
+      <c r="X3" s="271" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27">
+      <c r="Z4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27">
+      <c r="Z5" t="s">
+        <v>535</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27">
+      <c r="Z6" t="s">
+        <v>531</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27">
+      <c r="Z7" t="s">
+        <v>530</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>537</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CE14D2-6A31-4EE7-987E-9C9B413F95A3}">
   <dimension ref="B2:T21"/>
   <sheetViews>
@@ -17571,8 +17772,8 @@
     <col min="4" max="4" width="12.125" customWidth="1"/>
     <col min="5" max="5" width="17.25" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="16" max="16" width="13.125" style="288" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="13.125" style="288" customWidth="1"/>
+    <col min="16" max="16" width="13.125" style="274" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="13.125" style="274" customWidth="1"/>
     <col min="19" max="19" width="47.625" style="180" customWidth="1"/>
     <col min="20" max="20" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
@@ -17581,7 +17782,7 @@
       <c r="B2" t="s">
         <v>516</v>
       </c>
-      <c r="C2" s="290">
+      <c r="C2" s="276">
         <v>6.0221407599999999E+23</v>
       </c>
       <c r="S2" s="266"/>
@@ -17631,13 +17832,13 @@
       <c r="O5" s="169" t="s">
         <v>514</v>
       </c>
-      <c r="P5" s="287" t="s">
+      <c r="P5" s="273" t="s">
         <v>511</v>
       </c>
-      <c r="Q5" s="287" t="s">
+      <c r="Q5" s="273" t="s">
         <v>515</v>
       </c>
-      <c r="R5" s="289" t="s">
+      <c r="R5" s="275" t="s">
         <v>21</v>
       </c>
       <c r="S5" s="192" t="s">
@@ -17701,7 +17902,7 @@
         <f>C6*(Q6/P6)*(1E+27)/$C$2</f>
         <v>927.97418802324705</v>
       </c>
-      <c r="T6" s="286"/>
+      <c r="T6" s="272"/>
     </row>
     <row r="7" spans="2:20">
       <c r="B7" s="67"/>
@@ -18048,7 +18249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54734A79-229D-40A1-9EF2-2AA48E78AAE8}">
   <dimension ref="B2:R16"/>
   <sheetViews>
@@ -18067,11 +18268,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" s="181" customFormat="1">
-      <c r="C2" s="272" t="s">
+      <c r="C2" s="279" t="s">
         <v>396</v>
       </c>
-      <c r="D2" s="272"/>
-      <c r="E2" s="272"/>
+      <c r="D2" s="279"/>
+      <c r="E2" s="279"/>
       <c r="G2" s="161"/>
       <c r="H2" s="161"/>
       <c r="I2" s="161"/>
@@ -18998,11 +19199,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF9DD18-B806-45D2-93AF-832D747FF56C}">
   <dimension ref="A2:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -19028,11 +19229,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18">
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="278" t="s">
         <v>444</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="274"/>
+      <c r="C2" s="278"/>
+      <c r="D2" s="281"/>
       <c r="F2" s="238" t="s">
         <v>477</v>
       </c>
@@ -19694,11 +19895,11 @@
         <v>166</v>
       </c>
       <c r="F26" s="238">
-        <f>$D$26-$F$3</f>
+        <f t="shared" ref="F26:F33" si="2">$D$26-$F$3</f>
         <v>251</v>
       </c>
       <c r="G26" s="236">
-        <f>$D$26+$G$3</f>
+        <f t="shared" ref="G26:G33" si="3">$D$26+$G$3</f>
         <v>301</v>
       </c>
       <c r="H26" s="239" t="s">
@@ -19718,15 +19919,15 @@
       </c>
     </row>
     <row r="27" spans="1:18">
-      <c r="E27" s="291" t="s">
+      <c r="E27" s="277" t="s">
         <v>167</v>
       </c>
       <c r="F27" s="241">
-        <f>$D$26-$F$3</f>
+        <f t="shared" si="2"/>
         <v>251</v>
       </c>
       <c r="G27" s="239">
-        <f>$D$26+$G$3</f>
+        <f t="shared" si="3"/>
         <v>301</v>
       </c>
       <c r="H27" s="239" t="s">
@@ -19756,15 +19957,15 @@
     </row>
     <row r="28" spans="1:18" s="266" customFormat="1">
       <c r="D28" s="269"/>
-      <c r="E28" s="291" t="s">
+      <c r="E28" s="277" t="s">
         <v>167</v>
       </c>
       <c r="F28" s="268">
-        <f>$D$26-$F$3</f>
+        <f t="shared" si="2"/>
         <v>251</v>
       </c>
       <c r="G28" s="266">
-        <f>$D$26+$G$3</f>
+        <f t="shared" si="3"/>
         <v>301</v>
       </c>
       <c r="H28" s="266" t="s">
@@ -19797,15 +19998,15 @@
     </row>
     <row r="29" spans="1:18" s="266" customFormat="1">
       <c r="D29" s="269"/>
-      <c r="E29" s="291" t="s">
+      <c r="E29" s="277" t="s">
         <v>167</v>
       </c>
       <c r="F29" s="268">
-        <f>$D$26-$F$3</f>
+        <f t="shared" si="2"/>
         <v>251</v>
       </c>
       <c r="G29" s="266">
-        <f>$D$26+$G$3</f>
+        <f t="shared" si="3"/>
         <v>301</v>
       </c>
       <c r="H29" s="266" t="s">
@@ -19837,15 +20038,15 @@
     </row>
     <row r="30" spans="1:18" s="266" customFormat="1">
       <c r="D30" s="269"/>
-      <c r="E30" s="291" t="s">
+      <c r="E30" s="277" t="s">
         <v>167</v>
       </c>
       <c r="F30" s="268">
-        <f>$D$26-$F$3</f>
+        <f t="shared" si="2"/>
         <v>251</v>
       </c>
       <c r="G30" s="266">
-        <f>$D$26+$G$3</f>
+        <f t="shared" si="3"/>
         <v>301</v>
       </c>
       <c r="H30" s="266" t="s">
@@ -19877,15 +20078,15 @@
     </row>
     <row r="31" spans="1:18" s="266" customFormat="1">
       <c r="D31" s="269"/>
-      <c r="E31" s="291" t="s">
+      <c r="E31" s="277" t="s">
         <v>167</v>
       </c>
       <c r="F31" s="268">
-        <f>$D$26-$F$3</f>
+        <f t="shared" si="2"/>
         <v>251</v>
       </c>
       <c r="G31" s="266">
-        <f>$D$26+$G$3</f>
+        <f t="shared" si="3"/>
         <v>301</v>
       </c>
       <c r="H31" s="266" t="s">
@@ -19920,11 +20121,11 @@
         <v>168</v>
       </c>
       <c r="F32" s="249">
-        <f>$D$26-$F$3</f>
+        <f t="shared" si="2"/>
         <v>251</v>
       </c>
       <c r="G32" s="247">
-        <f>$D$26+$G$3</f>
+        <f t="shared" si="3"/>
         <v>301</v>
       </c>
       <c r="H32" s="247" t="s">
@@ -19958,11 +20159,11 @@
         <v>169</v>
       </c>
       <c r="F33" s="249">
-        <f>$D$26-$F$3</f>
+        <f t="shared" si="2"/>
         <v>251</v>
       </c>
       <c r="G33" s="247">
-        <f>$D$26+$G$3</f>
+        <f t="shared" si="3"/>
         <v>301</v>
       </c>
       <c r="H33" s="247" t="s">
@@ -20025,7 +20226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFF03F4-0D0E-4240-A36F-5BB31F518425}">
   <dimension ref="B2:E61"/>
   <sheetViews>
@@ -20900,7 +21101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB14C90-9A0C-E346-B9BD-40AE56D235C4}">
   <dimension ref="B1:BH45"/>
   <sheetViews>
@@ -20966,30 +21167,30 @@
       <c r="B2" s="82" t="s">
         <v>246</v>
       </c>
-      <c r="C2" s="284" t="s">
+      <c r="C2" s="291" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="284"/>
-      <c r="E2" s="284"/>
-      <c r="F2" s="284"/>
-      <c r="G2" s="284"/>
-      <c r="H2" s="283" t="s">
+      <c r="D2" s="291"/>
+      <c r="E2" s="291"/>
+      <c r="F2" s="291"/>
+      <c r="G2" s="291"/>
+      <c r="H2" s="290" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="283"/>
-      <c r="J2" s="283"/>
-      <c r="K2" s="283"/>
-      <c r="L2" s="283"/>
+      <c r="I2" s="290"/>
+      <c r="J2" s="290"/>
+      <c r="K2" s="290"/>
+      <c r="L2" s="290"/>
       <c r="N2" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="O2" s="284" t="s">
+      <c r="O2" s="291" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="284"/>
-      <c r="Q2" s="284"/>
-      <c r="R2" s="284"/>
-      <c r="S2" s="284"/>
+      <c r="P2" s="291"/>
+      <c r="Q2" s="291"/>
+      <c r="R2" s="291"/>
+      <c r="S2" s="291"/>
       <c r="T2" s="72"/>
       <c r="U2" s="72"/>
       <c r="V2" s="72"/>
@@ -20998,13 +21199,13 @@
       <c r="Z2" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="AA2" s="284" t="s">
+      <c r="AA2" s="291" t="s">
         <v>17</v>
       </c>
-      <c r="AB2" s="284"/>
-      <c r="AC2" s="284"/>
-      <c r="AD2" s="284"/>
-      <c r="AE2" s="284"/>
+      <c r="AB2" s="291"/>
+      <c r="AC2" s="291"/>
+      <c r="AD2" s="291"/>
+      <c r="AE2" s="291"/>
       <c r="AF2" s="72"/>
       <c r="AG2" s="72"/>
       <c r="AH2" s="72"/>
@@ -21013,13 +21214,13 @@
       <c r="AL2" s="77" t="s">
         <v>247</v>
       </c>
-      <c r="AM2" s="284" t="s">
+      <c r="AM2" s="291" t="s">
         <v>17</v>
       </c>
-      <c r="AN2" s="284"/>
-      <c r="AO2" s="284"/>
-      <c r="AP2" s="284"/>
-      <c r="AQ2" s="284"/>
+      <c r="AN2" s="291"/>
+      <c r="AO2" s="291"/>
+      <c r="AP2" s="291"/>
+      <c r="AQ2" s="291"/>
       <c r="AR2" s="72"/>
       <c r="AS2" s="72"/>
       <c r="AT2" s="72"/>
@@ -22159,33 +22360,33 @@
       <c r="B17" s="82" t="s">
         <v>246</v>
       </c>
-      <c r="C17" s="282" t="s">
+      <c r="C17" s="289" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="282"/>
-      <c r="E17" s="282"/>
-      <c r="F17" s="282"/>
-      <c r="G17" s="282"/>
+      <c r="D17" s="289"/>
+      <c r="E17" s="289"/>
+      <c r="F17" s="289"/>
+      <c r="G17" s="289"/>
       <c r="N17" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="O17" s="282" t="s">
+      <c r="O17" s="289" t="s">
         <v>17</v>
       </c>
-      <c r="P17" s="282"/>
-      <c r="Q17" s="282"/>
-      <c r="R17" s="282"/>
-      <c r="S17" s="282"/>
+      <c r="P17" s="289"/>
+      <c r="Q17" s="289"/>
+      <c r="R17" s="289"/>
+      <c r="S17" s="289"/>
       <c r="AL17" s="77" t="s">
         <v>247</v>
       </c>
-      <c r="AM17" s="284" t="s">
+      <c r="AM17" s="291" t="s">
         <v>17</v>
       </c>
-      <c r="AN17" s="284"/>
-      <c r="AO17" s="284"/>
-      <c r="AP17" s="284"/>
-      <c r="AQ17" s="284"/>
+      <c r="AN17" s="291"/>
+      <c r="AO17" s="291"/>
+      <c r="AP17" s="291"/>
+      <c r="AQ17" s="291"/>
       <c r="AR17" s="72"/>
       <c r="AS17" s="72"/>
       <c r="AT17" s="72"/>
@@ -22806,40 +23007,40 @@
       <c r="B32" s="82" t="s">
         <v>246</v>
       </c>
-      <c r="C32" s="284" t="s">
+      <c r="C32" s="291" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="284"/>
-      <c r="E32" s="284"/>
-      <c r="F32" s="284"/>
-      <c r="G32" s="284"/>
-      <c r="H32" s="283" t="s">
+      <c r="D32" s="291"/>
+      <c r="E32" s="291"/>
+      <c r="F32" s="291"/>
+      <c r="G32" s="291"/>
+      <c r="H32" s="290" t="s">
         <v>18</v>
       </c>
-      <c r="I32" s="283"/>
-      <c r="J32" s="283"/>
-      <c r="K32" s="283"/>
-      <c r="L32" s="283"/>
+      <c r="I32" s="290"/>
+      <c r="J32" s="290"/>
+      <c r="K32" s="290"/>
+      <c r="L32" s="290"/>
       <c r="N32" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="O32" s="282" t="s">
+      <c r="O32" s="289" t="s">
         <v>17</v>
       </c>
-      <c r="P32" s="282"/>
-      <c r="Q32" s="282"/>
-      <c r="R32" s="282"/>
-      <c r="S32" s="282"/>
+      <c r="P32" s="289"/>
+      <c r="Q32" s="289"/>
+      <c r="R32" s="289"/>
+      <c r="S32" s="289"/>
       <c r="AL32" s="77" t="s">
         <v>247</v>
       </c>
-      <c r="AM32" s="284" t="s">
+      <c r="AM32" s="291" t="s">
         <v>17</v>
       </c>
-      <c r="AN32" s="284"/>
-      <c r="AO32" s="284"/>
-      <c r="AP32" s="284"/>
-      <c r="AQ32" s="284"/>
+      <c r="AN32" s="291"/>
+      <c r="AO32" s="291"/>
+      <c r="AP32" s="291"/>
+      <c r="AQ32" s="291"/>
       <c r="AR32" s="72"/>
       <c r="AS32" s="72"/>
       <c r="AT32" s="72"/>
@@ -23415,7 +23616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BDCE98-34D0-4ABF-8516-E6ECC928D09D}">
   <dimension ref="B2:D32"/>
   <sheetViews>
@@ -23650,7 +23851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33EDBDFB-84C9-0D42-9872-D0E4DAFE61DB}">
   <dimension ref="B1:K10"/>
   <sheetViews>
@@ -23904,460 +24105,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E95DD15-E630-164A-9911-8F448DFCB0FA}">
-  <dimension ref="B1:Q33"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="4" width="10.875" style="14"/>
-    <col min="5" max="5" width="10.875" style="27"/>
-    <col min="6" max="6" width="10.875" style="29"/>
-    <col min="7" max="7" width="12.125" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.125" style="27" customWidth="1"/>
-    <col min="9" max="9" width="15.625" style="36" customWidth="1"/>
-    <col min="10" max="11" width="10.875" style="31"/>
-    <col min="12" max="16384" width="10.875" style="14"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:17">
-      <c r="I1" s="285" t="s">
-        <v>119</v>
-      </c>
-      <c r="J1" s="285"/>
-      <c r="K1" s="285"/>
-      <c r="L1" s="285"/>
-      <c r="M1" s="285"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="285"/>
-    </row>
-    <row r="2" spans="2:17">
-      <c r="C2" s="271" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="271"/>
-      <c r="F2" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="I2" s="285" t="s">
-        <v>117</v>
-      </c>
-      <c r="J2" s="285"/>
-      <c r="K2" s="285"/>
-      <c r="L2" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" s="15" customFormat="1">
-      <c r="B3" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="I3" s="35"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="M3" s="15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17">
-      <c r="B4" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="14">
-        <v>3.01</v>
-      </c>
-      <c r="D4" s="14">
-        <v>770</v>
-      </c>
-      <c r="E4" s="27">
-        <v>7.8543099999999999</v>
-      </c>
-      <c r="F4" s="29">
-        <f>1/332</f>
-        <v>3.0120481927710845E-3</v>
-      </c>
-      <c r="G4" s="37">
-        <f>2*PI()*F4*C4*1000/(D4*E4)</f>
-        <v>9.4191023645437116E-3</v>
-      </c>
-      <c r="H4" s="34">
-        <f>D4*E4*E4*(0.000001)/(C4*0.001)</f>
-        <v>15.78121026365349</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17">
-      <c r="B5" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="29">
-        <f>1/300</f>
-        <v>3.3333333333333335E-3</v>
-      </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="34"/>
-    </row>
-    <row r="6" spans="2:17">
-      <c r="B6" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="34"/>
-    </row>
-    <row r="7" spans="2:17">
-      <c r="B7" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="34"/>
-    </row>
-    <row r="8" spans="2:17">
-      <c r="G8" s="37"/>
-      <c r="H8" s="34"/>
-    </row>
-    <row r="9" spans="2:17" s="15" customFormat="1">
-      <c r="E9" s="28"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-    </row>
-    <row r="10" spans="2:17">
-      <c r="B10" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="I10" s="36">
-        <f>1000/587.575</f>
-        <v>1.7019103944177338</v>
-      </c>
-      <c r="J10" s="31">
-        <f>1000/393.087</f>
-        <v>2.5439660940198991</v>
-      </c>
-      <c r="K10" s="31">
-        <f>1000/524.365</f>
-        <v>1.9070685495790145</v>
-      </c>
-      <c r="L10" s="14">
-        <f>1000/429.592</f>
-        <v>2.3277900892009162</v>
-      </c>
-      <c r="M10" s="14">
-        <f>1000/471.267</f>
-        <v>2.1219393677045071</v>
-      </c>
-      <c r="P10" s="29">
-        <f>SUM(I10:O10)/5</f>
-        <v>2.1205348989844142</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17">
-      <c r="G11" s="31">
-        <v>2E-3</v>
-      </c>
-      <c r="I11" s="36">
-        <f>1000/ 539.436</f>
-        <v>1.8537880304614447</v>
-      </c>
-      <c r="J11" s="31">
-        <f>1000/427.898</f>
-        <v>2.3370055480511711</v>
-      </c>
-      <c r="K11" s="31">
-        <f>1000/482.665</f>
-        <v>2.0718303585302436</v>
-      </c>
-      <c r="L11" s="14">
-        <f>1000/425.574</f>
-        <v>2.3497676079835705</v>
-      </c>
-      <c r="M11" s="14">
-        <f>1000/450.603</f>
-        <v>2.2192484293269241</v>
-      </c>
-      <c r="P11" s="29">
-        <f>SUM(I11:O11)/5</f>
-        <v>2.1663279948706711</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17">
-      <c r="G12" s="31">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="I12" s="36">
-        <f>1000/511.599</f>
-        <v>1.9546558926033866</v>
-      </c>
-      <c r="J12" s="31">
-        <f>1000/463.492</f>
-        <v>2.1575345421280194</v>
-      </c>
-      <c r="K12" s="31">
-        <f>1000/428.438</f>
-        <v>2.3340600040145834</v>
-      </c>
-      <c r="L12" s="14">
-        <f>1000/484.767</f>
-        <v>2.0628466871713629</v>
-      </c>
-      <c r="M12" s="14">
-        <f>1000/456.876</f>
-        <v>2.1887776989817809</v>
-      </c>
-      <c r="P12" s="29">
-        <f>SUM(I12:O12)/5</f>
-        <v>2.1395749649798268</v>
-      </c>
-      <c r="Q12" s="29"/>
-    </row>
-    <row r="13" spans="2:17">
-      <c r="G13" s="31">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="I13" s="36">
-        <f>1000/468.013</f>
-        <v>2.1366927841747985</v>
-      </c>
-      <c r="J13" s="31">
-        <f>1000/484.467</f>
-        <v>2.0641240786266146</v>
-      </c>
-      <c r="K13" s="31">
-        <f>1000/495.902</f>
-        <v>2.01652745905441</v>
-      </c>
-      <c r="L13" s="14">
-        <f>1000/476.432</f>
-        <v>2.0989354199549988</v>
-      </c>
-      <c r="M13" s="14">
-        <f>1000/480.887</f>
-        <v>2.0794906079806692</v>
-      </c>
-      <c r="P13" s="29">
-        <f>SUM(I13:O13)/5</f>
-        <v>2.0791540699582982</v>
-      </c>
-      <c r="Q13" s="29"/>
-    </row>
-    <row r="14" spans="2:17">
-      <c r="G14" s="31">
-        <v>1.2E-2</v>
-      </c>
-      <c r="I14" s="36">
-        <f>1000/561.938</f>
-        <v>1.7795557517021452</v>
-      </c>
-      <c r="J14" s="31">
-        <f>1000/567.598</f>
-        <v>1.7618102953146417</v>
-      </c>
-      <c r="K14" s="31">
-        <f>1000/573.548</f>
-        <v>1.7435332352305299</v>
-      </c>
-      <c r="L14" s="14">
-        <f>1000/580.314</f>
-        <v>1.7232050234872847</v>
-      </c>
-      <c r="M14" s="14">
-        <f>1000/559.257</f>
-        <v>1.7880866935952524</v>
-      </c>
-      <c r="P14" s="29">
-        <f>SUM(I14:O14)/5</f>
-        <v>1.7592381998659707</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17">
-      <c r="I15" s="36" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17">
-      <c r="I16" s="36" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="B17" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="31">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="I17" s="36">
-        <f>1000/447.965</f>
-        <v>2.232317256928555</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="G18" s="31">
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="I18" s="36">
-        <f>1000/462.314</f>
-        <v>2.1630320518089436</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="G19" s="31">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="I19" s="36">
-        <f>1000/473.077</f>
-        <v>2.1138207945006839</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9">
-      <c r="G20" s="31">
-        <v>7.1000000000000004E-3</v>
-      </c>
-      <c r="I20" s="36">
-        <f>1000/490.985</f>
-        <v>2.0367220994531401</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9">
-      <c r="G21" s="31">
-        <v>0.01</v>
-      </c>
-      <c r="I21" s="36">
-        <f>1000/537.393</f>
-        <v>1.8608355523797295</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9">
-      <c r="G22" s="31">
-        <v>1.41E-2</v>
-      </c>
-      <c r="I22" s="36">
-        <f>1000/618.682</f>
-        <v>1.6163392502125487</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9">
-      <c r="G23" s="31">
-        <v>0.02</v>
-      </c>
-      <c r="I23" s="36">
-        <f>1000/768.18</f>
-        <v>1.3017782290608972</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9">
-      <c r="I25" s="36" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9">
-      <c r="I26" s="36" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9">
-      <c r="G27" s="31">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="I27" s="36">
-        <f>1000/450.232</f>
-        <v>2.2210771335666943</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9">
-      <c r="G28" s="31">
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="I28" s="36">
-        <f>1000/467.009</f>
-        <v>2.1412863563657232</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9">
-      <c r="G29" s="31">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="I29" s="36">
-        <f>1000/468.867</f>
-        <v>2.132800986207176</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9">
-      <c r="G30" s="31">
-        <v>7.1000000000000004E-3</v>
-      </c>
-      <c r="I30" s="36">
-        <f>1000/490.496</f>
-        <v>2.0387526096033404</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9">
-      <c r="G31" s="31">
-        <v>0.01</v>
-      </c>
-      <c r="I31" s="36">
-        <f>1000/523.234</f>
-        <v>1.9111907865314561</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9">
-      <c r="G32" s="31">
-        <v>1.41E-2</v>
-      </c>
-      <c r="I32" s="36">
-        <f>1000/599.115</f>
-        <v>1.6691286313979787</v>
-      </c>
-    </row>
-    <row r="33" spans="7:9">
-      <c r="G33" s="31">
-        <v>0.02</v>
-      </c>
-      <c r="I33" s="36">
-        <f>1000/741.736</f>
-        <v>1.348188573832199</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="I1:O1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -24542,6 +24289,460 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E95DD15-E630-164A-9911-8F448DFCB0FA}">
+  <dimension ref="B1:Q33"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="4" width="10.875" style="14"/>
+    <col min="5" max="5" width="10.875" style="27"/>
+    <col min="6" max="6" width="10.875" style="29"/>
+    <col min="7" max="7" width="12.125" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="27" customWidth="1"/>
+    <col min="9" max="9" width="15.625" style="36" customWidth="1"/>
+    <col min="10" max="11" width="10.875" style="31"/>
+    <col min="12" max="16384" width="10.875" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17">
+      <c r="I1" s="292" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="292"/>
+      <c r="K1" s="292"/>
+      <c r="L1" s="292"/>
+      <c r="M1" s="292"/>
+      <c r="N1" s="292"/>
+      <c r="O1" s="292"/>
+    </row>
+    <row r="2" spans="2:17">
+      <c r="C2" s="278" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="278"/>
+      <c r="F2" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="292" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2" s="292"/>
+      <c r="K2" s="292"/>
+      <c r="L2" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" s="15" customFormat="1">
+      <c r="B3" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" s="35"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="M3" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="B4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="14">
+        <v>3.01</v>
+      </c>
+      <c r="D4" s="14">
+        <v>770</v>
+      </c>
+      <c r="E4" s="27">
+        <v>7.8543099999999999</v>
+      </c>
+      <c r="F4" s="29">
+        <f>1/332</f>
+        <v>3.0120481927710845E-3</v>
+      </c>
+      <c r="G4" s="37">
+        <f>2*PI()*F4*C4*1000/(D4*E4)</f>
+        <v>9.4191023645437116E-3</v>
+      </c>
+      <c r="H4" s="34">
+        <f>D4*E4*E4*(0.000001)/(C4*0.001)</f>
+        <v>15.78121026365349</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="B5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="29">
+        <f>1/300</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="G5" s="37"/>
+      <c r="H5" s="34"/>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="B6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="37"/>
+      <c r="H6" s="34"/>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="B7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="37"/>
+      <c r="H7" s="34"/>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="G8" s="37"/>
+      <c r="H8" s="34"/>
+    </row>
+    <row r="9" spans="2:17" s="15" customFormat="1">
+      <c r="E9" s="28"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="B10" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="I10" s="36">
+        <f>1000/587.575</f>
+        <v>1.7019103944177338</v>
+      </c>
+      <c r="J10" s="31">
+        <f>1000/393.087</f>
+        <v>2.5439660940198991</v>
+      </c>
+      <c r="K10" s="31">
+        <f>1000/524.365</f>
+        <v>1.9070685495790145</v>
+      </c>
+      <c r="L10" s="14">
+        <f>1000/429.592</f>
+        <v>2.3277900892009162</v>
+      </c>
+      <c r="M10" s="14">
+        <f>1000/471.267</f>
+        <v>2.1219393677045071</v>
+      </c>
+      <c r="P10" s="29">
+        <f>SUM(I10:O10)/5</f>
+        <v>2.1205348989844142</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="G11" s="31">
+        <v>2E-3</v>
+      </c>
+      <c r="I11" s="36">
+        <f>1000/ 539.436</f>
+        <v>1.8537880304614447</v>
+      </c>
+      <c r="J11" s="31">
+        <f>1000/427.898</f>
+        <v>2.3370055480511711</v>
+      </c>
+      <c r="K11" s="31">
+        <f>1000/482.665</f>
+        <v>2.0718303585302436</v>
+      </c>
+      <c r="L11" s="14">
+        <f>1000/425.574</f>
+        <v>2.3497676079835705</v>
+      </c>
+      <c r="M11" s="14">
+        <f>1000/450.603</f>
+        <v>2.2192484293269241</v>
+      </c>
+      <c r="P11" s="29">
+        <f>SUM(I11:O11)/5</f>
+        <v>2.1663279948706711</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="G12" s="31">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I12" s="36">
+        <f>1000/511.599</f>
+        <v>1.9546558926033866</v>
+      </c>
+      <c r="J12" s="31">
+        <f>1000/463.492</f>
+        <v>2.1575345421280194</v>
+      </c>
+      <c r="K12" s="31">
+        <f>1000/428.438</f>
+        <v>2.3340600040145834</v>
+      </c>
+      <c r="L12" s="14">
+        <f>1000/484.767</f>
+        <v>2.0628466871713629</v>
+      </c>
+      <c r="M12" s="14">
+        <f>1000/456.876</f>
+        <v>2.1887776989817809</v>
+      </c>
+      <c r="P12" s="29">
+        <f>SUM(I12:O12)/5</f>
+        <v>2.1395749649798268</v>
+      </c>
+      <c r="Q12" s="29"/>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="G13" s="31">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I13" s="36">
+        <f>1000/468.013</f>
+        <v>2.1366927841747985</v>
+      </c>
+      <c r="J13" s="31">
+        <f>1000/484.467</f>
+        <v>2.0641240786266146</v>
+      </c>
+      <c r="K13" s="31">
+        <f>1000/495.902</f>
+        <v>2.01652745905441</v>
+      </c>
+      <c r="L13" s="14">
+        <f>1000/476.432</f>
+        <v>2.0989354199549988</v>
+      </c>
+      <c r="M13" s="14">
+        <f>1000/480.887</f>
+        <v>2.0794906079806692</v>
+      </c>
+      <c r="P13" s="29">
+        <f>SUM(I13:O13)/5</f>
+        <v>2.0791540699582982</v>
+      </c>
+      <c r="Q13" s="29"/>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="G14" s="31">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I14" s="36">
+        <f>1000/561.938</f>
+        <v>1.7795557517021452</v>
+      </c>
+      <c r="J14" s="31">
+        <f>1000/567.598</f>
+        <v>1.7618102953146417</v>
+      </c>
+      <c r="K14" s="31">
+        <f>1000/573.548</f>
+        <v>1.7435332352305299</v>
+      </c>
+      <c r="L14" s="14">
+        <f>1000/580.314</f>
+        <v>1.7232050234872847</v>
+      </c>
+      <c r="M14" s="14">
+        <f>1000/559.257</f>
+        <v>1.7880866935952524</v>
+      </c>
+      <c r="P14" s="29">
+        <f>SUM(I14:O14)/5</f>
+        <v>1.7592381998659707</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="I15" s="36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="I16" s="36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="31">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="I17" s="36">
+        <f>1000/447.965</f>
+        <v>2.232317256928555</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="G18" s="31">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="I18" s="36">
+        <f>1000/462.314</f>
+        <v>2.1630320518089436</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="G19" s="31">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I19" s="36">
+        <f>1000/473.077</f>
+        <v>2.1138207945006839</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="G20" s="31">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="I20" s="36">
+        <f>1000/490.985</f>
+        <v>2.0367220994531401</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="G21" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="I21" s="36">
+        <f>1000/537.393</f>
+        <v>1.8608355523797295</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="G22" s="31">
+        <v>1.41E-2</v>
+      </c>
+      <c r="I22" s="36">
+        <f>1000/618.682</f>
+        <v>1.6163392502125487</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="G23" s="31">
+        <v>0.02</v>
+      </c>
+      <c r="I23" s="36">
+        <f>1000/768.18</f>
+        <v>1.3017782290608972</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="I25" s="36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="I26" s="36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="G27" s="31">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="I27" s="36">
+        <f>1000/450.232</f>
+        <v>2.2210771335666943</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="G28" s="31">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="I28" s="36">
+        <f>1000/467.009</f>
+        <v>2.1412863563657232</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="G29" s="31">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I29" s="36">
+        <f>1000/468.867</f>
+        <v>2.132800986207176</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="G30" s="31">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="I30" s="36">
+        <f>1000/490.496</f>
+        <v>2.0387526096033404</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="G31" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="I31" s="36">
+        <f>1000/523.234</f>
+        <v>1.9111907865314561</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="G32" s="31">
+        <v>1.41E-2</v>
+      </c>
+      <c r="I32" s="36">
+        <f>1000/599.115</f>
+        <v>1.6691286313979787</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9">
+      <c r="G33" s="31">
+        <v>0.02</v>
+      </c>
+      <c r="I33" s="36">
+        <f>1000/741.736</f>
+        <v>1.348188573832199</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="I1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C044A9FB-F8D3-4917-BFAB-FBE43DD433AF}">
   <dimension ref="B3:BH17"/>
   <sheetViews>
@@ -24608,51 +24809,51 @@
       <c r="F4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="283" t="s">
+      <c r="H4" s="290" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="283"/>
-      <c r="J4" s="283"/>
-      <c r="K4" s="283"/>
-      <c r="L4" s="283"/>
+      <c r="I4" s="290"/>
+      <c r="J4" s="290"/>
+      <c r="K4" s="290"/>
+      <c r="L4" s="290"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
-      <c r="T4" s="283" t="s">
+      <c r="T4" s="290" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="283"/>
-      <c r="V4" s="283"/>
-      <c r="W4" s="283"/>
-      <c r="X4" s="283"/>
+      <c r="U4" s="290"/>
+      <c r="V4" s="290"/>
+      <c r="W4" s="290"/>
+      <c r="X4" s="290"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="7"/>
-      <c r="AF4" s="283" t="s">
+      <c r="AF4" s="290" t="s">
         <v>18</v>
       </c>
-      <c r="AG4" s="283"/>
-      <c r="AH4" s="283"/>
-      <c r="AI4" s="283"/>
-      <c r="AJ4" s="283"/>
+      <c r="AG4" s="290"/>
+      <c r="AH4" s="290"/>
+      <c r="AI4" s="290"/>
+      <c r="AJ4" s="290"/>
       <c r="AN4" s="10"/>
       <c r="AP4" s="7"/>
-      <c r="AR4" s="283" t="s">
+      <c r="AR4" s="290" t="s">
         <v>18</v>
       </c>
-      <c r="AS4" s="283"/>
-      <c r="AT4" s="283"/>
-      <c r="AU4" s="283"/>
-      <c r="AV4" s="283"/>
+      <c r="AS4" s="290"/>
+      <c r="AT4" s="290"/>
+      <c r="AU4" s="290"/>
+      <c r="AV4" s="290"/>
       <c r="BB4" s="7"/>
-      <c r="BD4" s="283" t="s">
+      <c r="BD4" s="290" t="s">
         <v>18</v>
       </c>
-      <c r="BE4" s="283"/>
-      <c r="BF4" s="283"/>
-      <c r="BG4" s="283"/>
-      <c r="BH4" s="283"/>
+      <c r="BE4" s="290"/>
+      <c r="BF4" s="290"/>
+      <c r="BG4" s="290"/>
+      <c r="BH4" s="290"/>
     </row>
     <row r="5" spans="2:60" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="B5" s="12" t="s">
@@ -25735,23 +25936,23 @@
       <c r="T2" s="260"/>
     </row>
     <row r="3" spans="2:24">
-      <c r="J3" s="271" t="s">
+      <c r="J3" s="278" t="s">
         <v>289</v>
       </c>
-      <c r="K3" s="271"/>
-      <c r="N3" s="271" t="s">
+      <c r="K3" s="278"/>
+      <c r="N3" s="278" t="s">
         <v>78</v>
       </c>
-      <c r="O3" s="271"/>
-      <c r="Q3" s="271" t="s">
+      <c r="O3" s="278"/>
+      <c r="Q3" s="278" t="s">
         <v>99</v>
       </c>
-      <c r="R3" s="271"/>
-      <c r="S3" s="271"/>
-      <c r="T3" s="271"/>
-      <c r="U3" s="271"/>
-      <c r="V3" s="271"/>
-      <c r="W3" s="271"/>
+      <c r="R3" s="278"/>
+      <c r="S3" s="278"/>
+      <c r="T3" s="278"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
     </row>
     <row r="4" spans="2:24" s="15" customFormat="1">
       <c r="B4" s="21" t="s">
@@ -27408,23 +27609,23 @@
       <c r="U2"/>
     </row>
     <row r="3" spans="2:24">
-      <c r="K3" s="271" t="s">
+      <c r="K3" s="278" t="s">
         <v>289</v>
       </c>
-      <c r="L3" s="271"/>
-      <c r="O3" s="271" t="s">
+      <c r="L3" s="278"/>
+      <c r="O3" s="278" t="s">
         <v>78</v>
       </c>
-      <c r="P3" s="271"/>
-      <c r="R3" s="271" t="s">
+      <c r="P3" s="278"/>
+      <c r="R3" s="278" t="s">
         <v>99</v>
       </c>
-      <c r="S3" s="271"/>
-      <c r="T3" s="271"/>
-      <c r="U3" s="271"/>
-      <c r="V3" s="271"/>
-      <c r="W3" s="271"/>
-      <c r="X3" s="271"/>
+      <c r="S3" s="278"/>
+      <c r="T3" s="278"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
     </row>
     <row r="4" spans="2:24" s="15" customFormat="1">
       <c r="B4" s="21" t="s">
@@ -29214,23 +29415,23 @@
       <c r="T2" s="152"/>
     </row>
     <row r="3" spans="2:23">
-      <c r="J3" s="272" t="s">
+      <c r="J3" s="279" t="s">
         <v>289</v>
       </c>
-      <c r="K3" s="272"/>
-      <c r="N3" s="272" t="s">
+      <c r="K3" s="279"/>
+      <c r="N3" s="279" t="s">
         <v>78</v>
       </c>
-      <c r="O3" s="272"/>
-      <c r="Q3" s="272" t="s">
+      <c r="O3" s="279"/>
+      <c r="Q3" s="279" t="s">
         <v>99</v>
       </c>
-      <c r="R3" s="272"/>
-      <c r="S3" s="272"/>
-      <c r="T3" s="272"/>
-      <c r="U3" s="272"/>
-      <c r="V3" s="272"/>
-      <c r="W3" s="272"/>
+      <c r="R3" s="279"/>
+      <c r="S3" s="279"/>
+      <c r="T3" s="279"/>
+      <c r="U3" s="279"/>
+      <c r="V3" s="279"/>
+      <c r="W3" s="279"/>
     </row>
     <row r="4" spans="2:23" s="158" customFormat="1">
       <c r="B4" s="162" t="s">
@@ -30171,19 +30372,19 @@
       <c r="O3" s="146" t="s">
         <v>83</v>
       </c>
-      <c r="Q3" s="273" t="s">
+      <c r="Q3" s="280" t="s">
         <v>78</v>
       </c>
-      <c r="R3" s="273"/>
-      <c r="S3" s="273"/>
-      <c r="U3" s="273" t="s">
+      <c r="R3" s="280"/>
+      <c r="S3" s="280"/>
+      <c r="U3" s="280" t="s">
         <v>99</v>
       </c>
-      <c r="V3" s="273"/>
-      <c r="W3" s="273"/>
-      <c r="X3" s="273"/>
-      <c r="Y3" s="273"/>
-      <c r="Z3" s="273"/>
+      <c r="V3" s="280"/>
+      <c r="W3" s="280"/>
+      <c r="X3" s="280"/>
+      <c r="Y3" s="280"/>
+      <c r="Z3" s="280"/>
     </row>
     <row r="4" spans="2:27" hidden="1">
       <c r="B4" s="147" t="s">
@@ -30544,23 +30745,23 @@
     <row r="10" spans="2:27">
       <c r="E10" s="146"/>
       <c r="F10" s="146"/>
-      <c r="J10" s="273" t="s">
+      <c r="J10" s="280" t="s">
         <v>289</v>
       </c>
-      <c r="K10" s="273"/>
-      <c r="N10" s="273" t="s">
+      <c r="K10" s="280"/>
+      <c r="N10" s="280" t="s">
         <v>78</v>
       </c>
-      <c r="O10" s="273"/>
-      <c r="Q10" s="273" t="s">
+      <c r="O10" s="280"/>
+      <c r="Q10" s="280" t="s">
         <v>99</v>
       </c>
-      <c r="R10" s="273"/>
-      <c r="S10" s="273"/>
-      <c r="T10" s="273"/>
-      <c r="U10" s="273"/>
-      <c r="V10" s="273"/>
-      <c r="W10" s="273"/>
+      <c r="R10" s="280"/>
+      <c r="S10" s="280"/>
+      <c r="T10" s="280"/>
+      <c r="U10" s="280"/>
+      <c r="V10" s="280"/>
+      <c r="W10" s="280"/>
       <c r="X10" s="146"/>
       <c r="AA10" s="146"/>
     </row>
@@ -31230,19 +31431,19 @@
       <c r="O3" s="134" t="s">
         <v>83</v>
       </c>
-      <c r="Q3" s="273" t="s">
+      <c r="Q3" s="280" t="s">
         <v>78</v>
       </c>
-      <c r="R3" s="273"/>
-      <c r="S3" s="273"/>
-      <c r="U3" s="273" t="s">
+      <c r="R3" s="280"/>
+      <c r="S3" s="280"/>
+      <c r="U3" s="280" t="s">
         <v>99</v>
       </c>
-      <c r="V3" s="273"/>
-      <c r="W3" s="273"/>
-      <c r="X3" s="273"/>
-      <c r="Y3" s="273"/>
-      <c r="Z3" s="273"/>
+      <c r="V3" s="280"/>
+      <c r="W3" s="280"/>
+      <c r="X3" s="280"/>
+      <c r="Y3" s="280"/>
+      <c r="Z3" s="280"/>
     </row>
     <row r="4" spans="2:27" hidden="1">
       <c r="B4" s="129" t="s">
@@ -31603,23 +31804,23 @@
     <row r="10" spans="2:27">
       <c r="E10" s="134"/>
       <c r="F10" s="134"/>
-      <c r="J10" s="273" t="s">
+      <c r="J10" s="280" t="s">
         <v>289</v>
       </c>
-      <c r="K10" s="273"/>
-      <c r="N10" s="273" t="s">
+      <c r="K10" s="280"/>
+      <c r="N10" s="280" t="s">
         <v>78</v>
       </c>
-      <c r="O10" s="273"/>
-      <c r="Q10" s="273" t="s">
+      <c r="O10" s="280"/>
+      <c r="Q10" s="280" t="s">
         <v>99</v>
       </c>
-      <c r="R10" s="273"/>
-      <c r="S10" s="273"/>
-      <c r="T10" s="273"/>
-      <c r="U10" s="273"/>
-      <c r="V10" s="273"/>
-      <c r="W10" s="273"/>
+      <c r="R10" s="280"/>
+      <c r="S10" s="280"/>
+      <c r="T10" s="280"/>
+      <c r="U10" s="280"/>
+      <c r="V10" s="280"/>
+      <c r="W10" s="280"/>
       <c r="X10" s="134"/>
       <c r="AA10" s="134"/>
     </row>
@@ -32449,23 +32650,23 @@
     <row r="4" spans="2:27">
       <c r="E4" s="146"/>
       <c r="F4" s="146"/>
-      <c r="J4" s="273" t="s">
+      <c r="J4" s="280" t="s">
         <v>289</v>
       </c>
-      <c r="K4" s="273"/>
-      <c r="N4" s="273" t="s">
+      <c r="K4" s="280"/>
+      <c r="N4" s="280" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="273"/>
-      <c r="Q4" s="273" t="s">
+      <c r="O4" s="280"/>
+      <c r="Q4" s="280" t="s">
         <v>99</v>
       </c>
-      <c r="R4" s="273"/>
-      <c r="S4" s="273"/>
-      <c r="T4" s="273"/>
-      <c r="U4" s="273"/>
-      <c r="V4" s="273"/>
-      <c r="W4" s="273"/>
+      <c r="R4" s="280"/>
+      <c r="S4" s="280"/>
+      <c r="T4" s="280"/>
+      <c r="U4" s="280"/>
+      <c r="V4" s="280"/>
+      <c r="W4" s="280"/>
       <c r="X4" s="146"/>
       <c r="AA4" s="146"/>
     </row>
@@ -33270,20 +33471,20 @@
       <c r="Q3" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="S3" s="271" t="s">
+      <c r="S3" s="278" t="s">
         <v>78</v>
       </c>
-      <c r="T3" s="271"/>
-      <c r="U3" s="274"/>
-      <c r="W3" s="271" t="s">
+      <c r="T3" s="278"/>
+      <c r="U3" s="281"/>
+      <c r="W3" s="278" t="s">
         <v>99</v>
       </c>
-      <c r="X3" s="271"/>
-      <c r="Y3" s="271"/>
-      <c r="Z3" s="271"/>
-      <c r="AA3" s="271"/>
-      <c r="AB3" s="271"/>
-      <c r="AC3" s="271"/>
+      <c r="X3" s="278"/>
+      <c r="Y3" s="278"/>
+      <c r="Z3" s="278"/>
+      <c r="AA3" s="278"/>
+      <c r="AB3" s="278"/>
+      <c r="AC3" s="278"/>
     </row>
     <row r="4" spans="2:29" s="15" customFormat="1">
       <c r="B4" s="15" t="s">

</xml_diff>